<commit_message>
testing subpage - istqb
</commit_message>
<xml_diff>
--- a/PTAKI.xlsx
+++ b/PTAKI.xlsx
@@ -1,24 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tata\Desktop\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9139CF3C-B8D0-4C74-9C60-75BF9AB10ADA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
     <sheet name="Arkusz2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="124519"/>
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -26,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="59">
   <si>
     <t>1-spring</t>
   </si>
@@ -77,12 +71,6 @@
   </si>
   <si>
     <t>12-city greenery, park</t>
-  </si>
-  <si>
-    <t>16- rabbit, watermelon</t>
-  </si>
-  <si>
-    <t>17-goose, pumpkin</t>
   </si>
   <si>
     <t>20-white, bright</t>
@@ -187,9 +175,6 @@
     <t>Gołąb miejski (11)</t>
   </si>
   <si>
-    <t>Grzywarz (12)</t>
-  </si>
-  <si>
     <t>Sierpówka (13)</t>
   </si>
   <si>
@@ -199,20 +184,26 @@
     <t>Czapla biała (15)</t>
   </si>
   <si>
-    <t>18-big dog, sheepdog (100cm)</t>
-  </si>
-  <si>
     <t>Kapturka (16)</t>
   </si>
   <si>
     <t>Piegża (17)</t>
   </si>
+  <si>
+    <t>Grzywacz (12)</t>
+  </si>
+  <si>
+    <t>17-goose, pumpkin(40-90)</t>
+  </si>
+  <si>
+    <t>18-big dog, sheepdog (90-200cm)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -576,7 +567,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="Yu Gothic Light"/>
@@ -611,7 +602,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="Yu Gothic"/>
@@ -788,21 +779,21 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="C15:O48"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:H16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="4.42578125" style="1" customWidth="1"/>
     <col min="2" max="2" width="14.5703125" style="1" bestFit="1" customWidth="1"/>
@@ -815,7 +806,7 @@
     <col min="9" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="15" spans="9:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="9:15">
       <c r="I15" s="2"/>
       <c r="J15" s="2"/>
       <c r="K15" s="2"/>
@@ -824,7 +815,7 @@
       <c r="N15" s="2"/>
       <c r="O15" s="2"/>
     </row>
-    <row r="16" spans="9:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="9:15">
       <c r="I16" s="2"/>
       <c r="J16" s="2"/>
       <c r="K16" s="2"/>
@@ -833,7 +824,7 @@
       <c r="N16" s="2"/>
       <c r="O16" s="2"/>
     </row>
-    <row r="17" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:15">
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
@@ -848,7 +839,7 @@
       <c r="N17" s="2"/>
       <c r="O17" s="2"/>
     </row>
-    <row r="18" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:15">
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
@@ -863,7 +854,7 @@
       <c r="N18" s="2"/>
       <c r="O18" s="2"/>
     </row>
-    <row r="19" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:15">
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
@@ -878,7 +869,7 @@
       <c r="N19" s="2"/>
       <c r="O19" s="2"/>
     </row>
-    <row r="20" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:15">
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
@@ -893,7 +884,7 @@
       <c r="N20" s="2"/>
       <c r="O20" s="2"/>
     </row>
-    <row r="21" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="21" spans="3:15">
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
@@ -908,7 +899,7 @@
       <c r="N21" s="2"/>
       <c r="O21" s="2"/>
     </row>
-    <row r="22" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="22" spans="3:15">
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
@@ -923,7 +914,7 @@
       <c r="N22" s="2"/>
       <c r="O22" s="2"/>
     </row>
-    <row r="23" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="23" spans="3:15">
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
       <c r="E23" s="2"/>
@@ -938,7 +929,7 @@
       <c r="N23" s="2"/>
       <c r="O23" s="2"/>
     </row>
-    <row r="24" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="24" spans="3:15">
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
@@ -953,7 +944,7 @@
       <c r="N24" s="2"/>
       <c r="O24" s="2"/>
     </row>
-    <row r="25" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="25" spans="3:15">
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
       <c r="E25" s="2"/>
@@ -968,7 +959,7 @@
       <c r="N25" s="2"/>
       <c r="O25" s="2"/>
     </row>
-    <row r="26" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="26" spans="3:15">
       <c r="C26" s="2"/>
       <c r="D26" s="2"/>
       <c r="E26" s="2"/>
@@ -983,7 +974,7 @@
       <c r="N26" s="2"/>
       <c r="O26" s="2"/>
     </row>
-    <row r="27" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="27" spans="3:15">
       <c r="C27" s="2"/>
       <c r="D27" s="2"/>
       <c r="E27" s="2"/>
@@ -998,7 +989,7 @@
       <c r="N27" s="2"/>
       <c r="O27" s="2"/>
     </row>
-    <row r="28" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="28" spans="3:15">
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
@@ -1013,7 +1004,7 @@
       <c r="N28" s="2"/>
       <c r="O28" s="2"/>
     </row>
-    <row r="29" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="29" spans="3:15">
       <c r="C29" s="2"/>
       <c r="D29" s="2"/>
       <c r="E29" s="2"/>
@@ -1028,7 +1019,7 @@
       <c r="N29" s="2"/>
       <c r="O29" s="2"/>
     </row>
-    <row r="30" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="30" spans="3:15">
       <c r="C30" s="2"/>
       <c r="D30" s="2"/>
       <c r="E30" s="2"/>
@@ -1043,7 +1034,7 @@
       <c r="N30" s="2"/>
       <c r="O30" s="2"/>
     </row>
-    <row r="31" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="31" spans="3:15">
       <c r="C31" s="2"/>
       <c r="D31" s="2"/>
       <c r="E31" s="2"/>
@@ -1058,7 +1049,7 @@
       <c r="N31" s="2"/>
       <c r="O31" s="2"/>
     </row>
-    <row r="32" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="32" spans="3:15">
       <c r="C32" s="2"/>
       <c r="D32" s="2"/>
       <c r="E32" s="2"/>
@@ -1073,7 +1064,7 @@
       <c r="N32" s="2"/>
       <c r="O32" s="2"/>
     </row>
-    <row r="33" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="33" spans="3:15">
       <c r="C33" s="2"/>
       <c r="D33" s="2"/>
       <c r="E33" s="2"/>
@@ -1088,7 +1079,7 @@
       <c r="N33" s="2"/>
       <c r="O33" s="2"/>
     </row>
-    <row r="34" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="34" spans="3:15">
       <c r="C34" s="2"/>
       <c r="D34" s="2"/>
       <c r="E34" s="2"/>
@@ -1103,7 +1094,7 @@
       <c r="N34" s="2"/>
       <c r="O34" s="2"/>
     </row>
-    <row r="35" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="35" spans="3:15">
       <c r="C35" s="2"/>
       <c r="D35" s="2"/>
       <c r="E35" s="2"/>
@@ -1118,7 +1109,7 @@
       <c r="N35" s="2"/>
       <c r="O35" s="2"/>
     </row>
-    <row r="36" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="36" spans="3:15">
       <c r="C36" s="2"/>
       <c r="D36" s="2"/>
       <c r="E36" s="2"/>
@@ -1133,7 +1124,7 @@
       <c r="N36" s="2"/>
       <c r="O36" s="2"/>
     </row>
-    <row r="37" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="37" spans="3:15">
       <c r="C37" s="2"/>
       <c r="D37" s="2"/>
       <c r="E37" s="2"/>
@@ -1148,7 +1139,7 @@
       <c r="N37" s="2"/>
       <c r="O37" s="2"/>
     </row>
-    <row r="38" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="38" spans="3:15">
       <c r="C38" s="2"/>
       <c r="D38" s="2"/>
       <c r="E38" s="2"/>
@@ -1163,7 +1154,7 @@
       <c r="N38" s="2"/>
       <c r="O38" s="2"/>
     </row>
-    <row r="39" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="39" spans="3:15">
       <c r="C39" s="2"/>
       <c r="D39" s="2"/>
       <c r="E39" s="2"/>
@@ -1178,7 +1169,7 @@
       <c r="N39" s="2"/>
       <c r="O39" s="2"/>
     </row>
-    <row r="40" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="40" spans="3:15">
       <c r="C40" s="2"/>
       <c r="D40" s="2"/>
       <c r="E40" s="2"/>
@@ -1193,7 +1184,7 @@
       <c r="N40" s="2"/>
       <c r="O40" s="2"/>
     </row>
-    <row r="41" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="41" spans="3:15">
       <c r="C41" s="2"/>
       <c r="D41" s="2"/>
       <c r="E41" s="2"/>
@@ -1208,7 +1199,7 @@
       <c r="N41" s="2"/>
       <c r="O41" s="2"/>
     </row>
-    <row r="42" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="42" spans="3:15">
       <c r="C42" s="2"/>
       <c r="D42" s="2"/>
       <c r="E42" s="2"/>
@@ -1223,7 +1214,7 @@
       <c r="N42" s="2"/>
       <c r="O42" s="2"/>
     </row>
-    <row r="43" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="43" spans="3:15">
       <c r="C43" s="2"/>
       <c r="D43" s="2"/>
       <c r="E43" s="2"/>
@@ -1238,7 +1229,7 @@
       <c r="N43" s="2"/>
       <c r="O43" s="2"/>
     </row>
-    <row r="44" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="44" spans="3:15">
       <c r="C44" s="2"/>
       <c r="D44" s="2"/>
       <c r="E44" s="2"/>
@@ -1253,7 +1244,7 @@
       <c r="N44" s="2"/>
       <c r="O44" s="2"/>
     </row>
-    <row r="45" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="45" spans="3:15">
       <c r="C45" s="2"/>
       <c r="D45" s="2"/>
       <c r="E45" s="2"/>
@@ -1268,7 +1259,7 @@
       <c r="N45" s="2"/>
       <c r="O45" s="2"/>
     </row>
-    <row r="46" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="46" spans="3:15">
       <c r="C46" s="2"/>
       <c r="D46" s="2"/>
       <c r="E46" s="2"/>
@@ -1283,7 +1274,7 @@
       <c r="N46" s="2"/>
       <c r="O46" s="2"/>
     </row>
-    <row r="47" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="47" spans="3:15">
       <c r="C47" s="2"/>
       <c r="D47" s="2"/>
       <c r="E47" s="2"/>
@@ -1298,7 +1289,7 @@
       <c r="N47" s="2"/>
       <c r="O47" s="2"/>
     </row>
-    <row r="48" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="48" spans="3:15">
       <c r="C48" s="2"/>
       <c r="D48" s="2"/>
       <c r="E48" s="2"/>
@@ -1320,14 +1311,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D28F4F49-4A8D-4682-BCD7-181019FDAF25}">
-  <dimension ref="A1:DM57"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:DM56"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="11.25"/>
   <cols>
     <col min="1" max="1" width="28.5703125" style="4" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="4.7109375" style="5" customWidth="1"/>
@@ -1349,60 +1340,60 @@
     <col min="19" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:117" s="16" customFormat="1" ht="12" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:117" s="16" customFormat="1" ht="12" thickBot="1">
       <c r="C1" s="16" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="D1" s="16" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="E1" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="F1" s="45" t="s">
+        <v>52</v>
+      </c>
+      <c r="G1" s="45" t="s">
+        <v>53</v>
+      </c>
+      <c r="H1" s="58" t="s">
         <v>50</v>
       </c>
-      <c r="F1" s="45" t="s">
-        <v>55</v>
-      </c>
-      <c r="G1" s="45" t="s">
+      <c r="I1" s="58" t="s">
         <v>56</v>
       </c>
-      <c r="H1" s="58" t="s">
-        <v>52</v>
-      </c>
-      <c r="I1" s="58" t="s">
-        <v>53</v>
-      </c>
       <c r="J1" s="58" t="s">
+        <v>49</v>
+      </c>
+      <c r="K1" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="L1" s="45" t="s">
+        <v>43</v>
+      </c>
+      <c r="M1" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="N1" s="58" t="s">
+        <v>47</v>
+      </c>
+      <c r="O1" s="58" t="s">
         <v>51</v>
       </c>
-      <c r="K1" s="45" t="s">
+      <c r="P1" s="45" t="s">
         <v>42</v>
       </c>
-      <c r="L1" s="45" t="s">
-        <v>45</v>
-      </c>
-      <c r="M1" s="45" t="s">
+      <c r="Q1" s="45" t="s">
+        <v>37</v>
+      </c>
+      <c r="R1" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="N1" s="58" t="s">
-        <v>49</v>
-      </c>
-      <c r="O1" s="58" t="s">
-        <v>54</v>
-      </c>
-      <c r="P1" s="45" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q1" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="R1" s="16" t="s">
-        <v>43</v>
-      </c>
       <c r="S1" s="45" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="2" spans="1:117" s="9" customFormat="1" x14ac:dyDescent="0.2">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:117" s="9" customFormat="1">
       <c r="A2" s="7" t="s">
         <v>0</v>
       </c>
@@ -1525,7 +1516,7 @@
       <c r="DL2" s="23"/>
       <c r="DM2" s="23"/>
     </row>
-    <row r="3" spans="1:117" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:117" s="12" customFormat="1">
       <c r="A3" s="10" t="s">
         <v>1</v>
       </c>
@@ -1648,7 +1639,7 @@
       <c r="DL3" s="18"/>
       <c r="DM3" s="18"/>
     </row>
-    <row r="4" spans="1:117" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:117" s="12" customFormat="1">
       <c r="A4" s="10" t="s">
         <v>2</v>
       </c>
@@ -1771,7 +1762,7 @@
       <c r="DL4" s="18"/>
       <c r="DM4" s="18"/>
     </row>
-    <row r="5" spans="1:117" s="15" customFormat="1" ht="12" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:117" s="15" customFormat="1" ht="12" thickBot="1">
       <c r="A5" s="13" t="s">
         <v>3</v>
       </c>
@@ -1894,7 +1885,7 @@
       <c r="DL5" s="24"/>
       <c r="DM5" s="24"/>
     </row>
-    <row r="6" spans="1:117" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:117">
       <c r="A6" s="6" t="s">
         <v>11</v>
       </c>
@@ -2017,7 +2008,7 @@
       <c r="DL6" s="21"/>
       <c r="DM6" s="21"/>
     </row>
-    <row r="7" spans="1:117" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:117">
       <c r="A7" s="6" t="s">
         <v>6</v>
       </c>
@@ -2140,7 +2131,7 @@
       <c r="DL7" s="18"/>
       <c r="DM7" s="18"/>
     </row>
-    <row r="8" spans="1:117" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:117">
       <c r="A8" s="6" t="s">
         <v>12</v>
       </c>
@@ -2263,7 +2254,7 @@
       <c r="DL8" s="18"/>
       <c r="DM8" s="18"/>
     </row>
-    <row r="9" spans="1:117" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:117">
       <c r="A9" s="6" t="s">
         <v>13</v>
       </c>
@@ -2386,7 +2377,7 @@
       <c r="DL9" s="18"/>
       <c r="DM9" s="18"/>
     </row>
-    <row r="10" spans="1:117" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:117">
       <c r="A10" s="6" t="s">
         <v>14</v>
       </c>
@@ -2509,7 +2500,7 @@
       <c r="DL10" s="18"/>
       <c r="DM10" s="18"/>
     </row>
-    <row r="11" spans="1:117" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:117">
       <c r="A11" s="6" t="s">
         <v>8</v>
       </c>
@@ -2632,7 +2623,7 @@
       <c r="DL11" s="18"/>
       <c r="DM11" s="18"/>
     </row>
-    <row r="12" spans="1:117" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:117">
       <c r="A12" s="6" t="s">
         <v>15</v>
       </c>
@@ -2755,7 +2746,7 @@
       <c r="DL12" s="18"/>
       <c r="DM12" s="18"/>
     </row>
-    <row r="13" spans="1:117" ht="12" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:117" ht="12" thickBot="1">
       <c r="A13" s="6" t="s">
         <v>16</v>
       </c>
@@ -2878,9 +2869,9 @@
       <c r="DL13" s="25"/>
       <c r="DM13" s="25"/>
     </row>
-    <row r="14" spans="1:117" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:117" s="9" customFormat="1">
       <c r="A14" s="7" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B14" s="8">
         <v>13</v>
@@ -3001,9 +2992,9 @@
       <c r="DL14" s="23"/>
       <c r="DM14" s="23"/>
     </row>
-    <row r="15" spans="1:117" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:117" s="12" customFormat="1">
       <c r="A15" s="10" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B15" s="11">
         <v>14</v>
@@ -3124,9 +3115,9 @@
       <c r="DL15" s="18"/>
       <c r="DM15" s="18"/>
     </row>
-    <row r="16" spans="1:117" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:117" s="12" customFormat="1">
       <c r="A16" s="10" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B16" s="11">
         <v>15</v>
@@ -3247,12 +3238,12 @@
       <c r="DL16" s="18"/>
       <c r="DM16" s="18"/>
     </row>
-    <row r="17" spans="1:117" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:117" s="12" customFormat="1">
       <c r="A17" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="B17" s="11">
         <v>17</v>
-      </c>
-      <c r="B17" s="11">
-        <v>16</v>
       </c>
       <c r="C17" s="47"/>
       <c r="D17" s="47"/>
@@ -3260,7 +3251,7 @@
       <c r="F17" s="47"/>
       <c r="G17" s="47"/>
       <c r="H17" s="47"/>
-      <c r="I17" s="46"/>
+      <c r="I17" s="47"/>
       <c r="J17" s="47"/>
       <c r="K17" s="17"/>
       <c r="L17" s="17"/>
@@ -3370,18 +3361,18 @@
       <c r="DL17" s="18"/>
       <c r="DM17" s="18"/>
     </row>
-    <row r="18" spans="1:117" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="10" t="s">
+    <row r="18" spans="1:117" s="15" customFormat="1" ht="12" thickBot="1">
+      <c r="A18" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="B18" s="14">
         <v>18</v>
-      </c>
-      <c r="B18" s="11">
-        <v>17</v>
       </c>
       <c r="C18" s="47"/>
       <c r="D18" s="47"/>
-      <c r="E18" s="54"/>
-      <c r="F18" s="47"/>
-      <c r="G18" s="47"/>
+      <c r="E18" s="53"/>
+      <c r="F18" s="46"/>
+      <c r="G18" s="46"/>
       <c r="H18" s="47"/>
       <c r="I18" s="47"/>
       <c r="J18" s="47"/>
@@ -3394,380 +3385,380 @@
       <c r="Q18" s="18"/>
       <c r="R18" s="18"/>
       <c r="S18" s="18"/>
-      <c r="T18" s="17"/>
-      <c r="U18" s="17"/>
-      <c r="V18" s="17"/>
-      <c r="W18" s="17"/>
-      <c r="X18" s="18"/>
-      <c r="Y18" s="18"/>
-      <c r="Z18" s="18"/>
-      <c r="AA18" s="18"/>
-      <c r="AB18" s="18"/>
-      <c r="AC18" s="18"/>
-      <c r="AD18" s="18"/>
-      <c r="AE18" s="18"/>
-      <c r="AF18" s="18"/>
-      <c r="AG18" s="18"/>
-      <c r="AH18" s="18"/>
-      <c r="AI18" s="18"/>
-      <c r="AJ18" s="18"/>
-      <c r="AK18" s="18"/>
-      <c r="AL18" s="18"/>
-      <c r="AM18" s="18"/>
-      <c r="AN18" s="18"/>
-      <c r="AO18" s="18"/>
-      <c r="AP18" s="18"/>
-      <c r="AQ18" s="18"/>
-      <c r="AR18" s="18"/>
-      <c r="AS18" s="18"/>
-      <c r="AT18" s="18"/>
-      <c r="AU18" s="18"/>
-      <c r="AV18" s="18"/>
-      <c r="AW18" s="18"/>
-      <c r="AX18" s="18"/>
-      <c r="AY18" s="18"/>
-      <c r="AZ18" s="18"/>
-      <c r="BA18" s="18"/>
-      <c r="BB18" s="18"/>
-      <c r="BC18" s="18"/>
-      <c r="BD18" s="18"/>
-      <c r="BE18" s="18"/>
-      <c r="BF18" s="18"/>
-      <c r="BG18" s="18"/>
-      <c r="BH18" s="18"/>
-      <c r="BI18" s="18"/>
-      <c r="BJ18" s="18"/>
-      <c r="BK18" s="18"/>
-      <c r="BL18" s="18"/>
-      <c r="BM18" s="18"/>
-      <c r="BN18" s="18"/>
-      <c r="BO18" s="18"/>
-      <c r="BP18" s="18"/>
-      <c r="BQ18" s="18"/>
-      <c r="BR18" s="18"/>
-      <c r="BS18" s="18"/>
-      <c r="BT18" s="18"/>
-      <c r="BU18" s="18"/>
-      <c r="BV18" s="18"/>
-      <c r="BW18" s="18"/>
-      <c r="BX18" s="18"/>
-      <c r="BY18" s="18"/>
-      <c r="BZ18" s="18"/>
-      <c r="CA18" s="18"/>
-      <c r="CB18" s="18"/>
-      <c r="CC18" s="18"/>
-      <c r="CD18" s="18"/>
-      <c r="CE18" s="18"/>
-      <c r="CF18" s="18"/>
-      <c r="CG18" s="18"/>
-      <c r="CH18" s="18"/>
-      <c r="CI18" s="18"/>
-      <c r="CJ18" s="18"/>
-      <c r="CK18" s="18"/>
-      <c r="CL18" s="18"/>
-      <c r="CM18" s="18"/>
-      <c r="CN18" s="18"/>
-      <c r="CO18" s="18"/>
-      <c r="CP18" s="18"/>
-      <c r="CQ18" s="18"/>
-      <c r="CR18" s="18"/>
-      <c r="CS18" s="18"/>
-      <c r="CT18" s="18"/>
-      <c r="CU18" s="18"/>
-      <c r="CV18" s="18"/>
-      <c r="CW18" s="18"/>
-      <c r="CX18" s="18"/>
-      <c r="CY18" s="18"/>
-      <c r="CZ18" s="18"/>
-      <c r="DA18" s="18"/>
-      <c r="DB18" s="18"/>
-      <c r="DC18" s="18"/>
-      <c r="DD18" s="18"/>
-      <c r="DE18" s="18"/>
-      <c r="DF18" s="18"/>
-      <c r="DG18" s="18"/>
-      <c r="DH18" s="18"/>
-      <c r="DI18" s="18"/>
-      <c r="DJ18" s="18"/>
-      <c r="DK18" s="18"/>
-      <c r="DL18" s="18"/>
-      <c r="DM18" s="18"/>
-    </row>
-    <row r="19" spans="1:117" s="15" customFormat="1" ht="12" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="13" t="s">
-        <v>57</v>
-      </c>
-      <c r="B19" s="14">
-        <v>18</v>
+      <c r="T18" s="30"/>
+      <c r="U18" s="30"/>
+      <c r="V18" s="30"/>
+      <c r="W18" s="30"/>
+      <c r="X18" s="30"/>
+      <c r="Y18" s="24"/>
+      <c r="Z18" s="24"/>
+      <c r="AA18" s="24"/>
+      <c r="AB18" s="24"/>
+      <c r="AC18" s="24"/>
+      <c r="AD18" s="24"/>
+      <c r="AE18" s="24"/>
+      <c r="AF18" s="24"/>
+      <c r="AG18" s="24"/>
+      <c r="AH18" s="24"/>
+      <c r="AI18" s="24"/>
+      <c r="AJ18" s="24"/>
+      <c r="AK18" s="24"/>
+      <c r="AL18" s="24"/>
+      <c r="AM18" s="24"/>
+      <c r="AN18" s="24"/>
+      <c r="AO18" s="24"/>
+      <c r="AP18" s="24"/>
+      <c r="AQ18" s="24"/>
+      <c r="AR18" s="24"/>
+      <c r="AS18" s="24"/>
+      <c r="AT18" s="24"/>
+      <c r="AU18" s="24"/>
+      <c r="AV18" s="24"/>
+      <c r="AW18" s="24"/>
+      <c r="AX18" s="24"/>
+      <c r="AY18" s="24"/>
+      <c r="AZ18" s="24"/>
+      <c r="BA18" s="24"/>
+      <c r="BB18" s="24"/>
+      <c r="BC18" s="24"/>
+      <c r="BD18" s="24"/>
+      <c r="BE18" s="24"/>
+      <c r="BF18" s="24"/>
+      <c r="BG18" s="24"/>
+      <c r="BH18" s="24"/>
+      <c r="BI18" s="24"/>
+      <c r="BJ18" s="24"/>
+      <c r="BK18" s="24"/>
+      <c r="BL18" s="24"/>
+      <c r="BM18" s="24"/>
+      <c r="BN18" s="24"/>
+      <c r="BO18" s="24"/>
+      <c r="BP18" s="24"/>
+      <c r="BQ18" s="24"/>
+      <c r="BR18" s="24"/>
+      <c r="BS18" s="24"/>
+      <c r="BT18" s="24"/>
+      <c r="BU18" s="24"/>
+      <c r="BV18" s="24"/>
+      <c r="BW18" s="24"/>
+      <c r="BX18" s="24"/>
+      <c r="BY18" s="24"/>
+      <c r="BZ18" s="24"/>
+      <c r="CA18" s="24"/>
+      <c r="CB18" s="24"/>
+      <c r="CC18" s="24"/>
+      <c r="CD18" s="24"/>
+      <c r="CE18" s="24"/>
+      <c r="CF18" s="24"/>
+      <c r="CG18" s="24"/>
+      <c r="CH18" s="24"/>
+      <c r="CI18" s="24"/>
+      <c r="CJ18" s="24"/>
+      <c r="CK18" s="24"/>
+      <c r="CL18" s="24"/>
+      <c r="CM18" s="24"/>
+      <c r="CN18" s="24"/>
+      <c r="CO18" s="24"/>
+      <c r="CP18" s="24"/>
+      <c r="CQ18" s="24"/>
+      <c r="CR18" s="24"/>
+      <c r="CS18" s="24"/>
+      <c r="CT18" s="24"/>
+      <c r="CU18" s="24"/>
+      <c r="CV18" s="24"/>
+      <c r="CW18" s="24"/>
+      <c r="CX18" s="24"/>
+      <c r="CY18" s="24"/>
+      <c r="CZ18" s="24"/>
+      <c r="DA18" s="24"/>
+      <c r="DB18" s="24"/>
+      <c r="DC18" s="24"/>
+      <c r="DD18" s="24"/>
+      <c r="DE18" s="24"/>
+      <c r="DF18" s="24"/>
+      <c r="DG18" s="24"/>
+      <c r="DH18" s="24"/>
+      <c r="DI18" s="24"/>
+      <c r="DJ18" s="24"/>
+      <c r="DK18" s="24"/>
+      <c r="DL18" s="24"/>
+      <c r="DM18" s="24"/>
+    </row>
+    <row r="19" spans="1:117">
+      <c r="A19" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B19" s="5">
+        <v>19</v>
       </c>
       <c r="C19" s="47"/>
       <c r="D19" s="47"/>
-      <c r="E19" s="53"/>
-      <c r="F19" s="46"/>
-      <c r="G19" s="46"/>
+      <c r="E19" s="54"/>
+      <c r="F19" s="47"/>
+      <c r="G19" s="47"/>
       <c r="H19" s="47"/>
       <c r="I19" s="47"/>
       <c r="J19" s="47"/>
-      <c r="K19" s="17"/>
-      <c r="L19" s="17"/>
+      <c r="K19" s="52"/>
+      <c r="L19" s="51"/>
       <c r="M19" s="47"/>
       <c r="N19" s="47"/>
       <c r="O19" s="47"/>
-      <c r="P19" s="17"/>
-      <c r="Q19" s="18"/>
+      <c r="P19" s="51"/>
+      <c r="Q19" s="31"/>
       <c r="R19" s="18"/>
       <c r="S19" s="18"/>
-      <c r="T19" s="30"/>
-      <c r="U19" s="30"/>
-      <c r="V19" s="30"/>
-      <c r="W19" s="30"/>
-      <c r="X19" s="30"/>
-      <c r="Y19" s="24"/>
-      <c r="Z19" s="24"/>
-      <c r="AA19" s="24"/>
-      <c r="AB19" s="24"/>
-      <c r="AC19" s="24"/>
-      <c r="AD19" s="24"/>
-      <c r="AE19" s="24"/>
-      <c r="AF19" s="24"/>
-      <c r="AG19" s="24"/>
-      <c r="AH19" s="24"/>
-      <c r="AI19" s="24"/>
-      <c r="AJ19" s="24"/>
-      <c r="AK19" s="24"/>
-      <c r="AL19" s="24"/>
-      <c r="AM19" s="24"/>
-      <c r="AN19" s="24"/>
-      <c r="AO19" s="24"/>
-      <c r="AP19" s="24"/>
-      <c r="AQ19" s="24"/>
-      <c r="AR19" s="24"/>
-      <c r="AS19" s="24"/>
-      <c r="AT19" s="24"/>
-      <c r="AU19" s="24"/>
-      <c r="AV19" s="24"/>
-      <c r="AW19" s="24"/>
-      <c r="AX19" s="24"/>
-      <c r="AY19" s="24"/>
-      <c r="AZ19" s="24"/>
-      <c r="BA19" s="24"/>
-      <c r="BB19" s="24"/>
-      <c r="BC19" s="24"/>
-      <c r="BD19" s="24"/>
-      <c r="BE19" s="24"/>
-      <c r="BF19" s="24"/>
-      <c r="BG19" s="24"/>
-      <c r="BH19" s="24"/>
-      <c r="BI19" s="24"/>
-      <c r="BJ19" s="24"/>
-      <c r="BK19" s="24"/>
-      <c r="BL19" s="24"/>
-      <c r="BM19" s="24"/>
-      <c r="BN19" s="24"/>
-      <c r="BO19" s="24"/>
-      <c r="BP19" s="24"/>
-      <c r="BQ19" s="24"/>
-      <c r="BR19" s="24"/>
-      <c r="BS19" s="24"/>
-      <c r="BT19" s="24"/>
-      <c r="BU19" s="24"/>
-      <c r="BV19" s="24"/>
-      <c r="BW19" s="24"/>
-      <c r="BX19" s="24"/>
-      <c r="BY19" s="24"/>
-      <c r="BZ19" s="24"/>
-      <c r="CA19" s="24"/>
-      <c r="CB19" s="24"/>
-      <c r="CC19" s="24"/>
-      <c r="CD19" s="24"/>
-      <c r="CE19" s="24"/>
-      <c r="CF19" s="24"/>
-      <c r="CG19" s="24"/>
-      <c r="CH19" s="24"/>
-      <c r="CI19" s="24"/>
-      <c r="CJ19" s="24"/>
-      <c r="CK19" s="24"/>
-      <c r="CL19" s="24"/>
-      <c r="CM19" s="24"/>
-      <c r="CN19" s="24"/>
-      <c r="CO19" s="24"/>
-      <c r="CP19" s="24"/>
-      <c r="CQ19" s="24"/>
-      <c r="CR19" s="24"/>
-      <c r="CS19" s="24"/>
-      <c r="CT19" s="24"/>
-      <c r="CU19" s="24"/>
-      <c r="CV19" s="24"/>
-      <c r="CW19" s="24"/>
-      <c r="CX19" s="24"/>
-      <c r="CY19" s="24"/>
-      <c r="CZ19" s="24"/>
-      <c r="DA19" s="24"/>
-      <c r="DB19" s="24"/>
-      <c r="DC19" s="24"/>
-      <c r="DD19" s="24"/>
-      <c r="DE19" s="24"/>
-      <c r="DF19" s="24"/>
-      <c r="DG19" s="24"/>
-      <c r="DH19" s="24"/>
-      <c r="DI19" s="24"/>
-      <c r="DJ19" s="24"/>
-      <c r="DK19" s="24"/>
-      <c r="DL19" s="24"/>
-      <c r="DM19" s="24"/>
-    </row>
-    <row r="20" spans="1:117" x14ac:dyDescent="0.2">
+      <c r="T19" s="27"/>
+      <c r="U19" s="27"/>
+      <c r="V19" s="27"/>
+      <c r="W19" s="27"/>
+      <c r="X19" s="28"/>
+      <c r="Y19" s="21"/>
+      <c r="Z19" s="21"/>
+      <c r="AA19" s="21"/>
+      <c r="AB19" s="21"/>
+      <c r="AC19" s="21"/>
+      <c r="AD19" s="21"/>
+      <c r="AE19" s="21"/>
+      <c r="AF19" s="21"/>
+      <c r="AG19" s="21"/>
+      <c r="AH19" s="21"/>
+      <c r="AI19" s="21"/>
+      <c r="AJ19" s="21"/>
+      <c r="AK19" s="21"/>
+      <c r="AL19" s="21"/>
+      <c r="AM19" s="21"/>
+      <c r="AN19" s="21"/>
+      <c r="AO19" s="21"/>
+      <c r="AP19" s="21"/>
+      <c r="AQ19" s="21"/>
+      <c r="AR19" s="21"/>
+      <c r="AS19" s="21"/>
+      <c r="AT19" s="21"/>
+      <c r="AU19" s="21"/>
+      <c r="AV19" s="21"/>
+      <c r="AW19" s="21"/>
+      <c r="AX19" s="21"/>
+      <c r="AY19" s="21"/>
+      <c r="AZ19" s="21"/>
+      <c r="BA19" s="21"/>
+      <c r="BB19" s="21"/>
+      <c r="BC19" s="21"/>
+      <c r="BD19" s="21"/>
+      <c r="BE19" s="21"/>
+      <c r="BF19" s="21"/>
+      <c r="BG19" s="21"/>
+      <c r="BH19" s="21"/>
+      <c r="BI19" s="21"/>
+      <c r="BJ19" s="21"/>
+      <c r="BK19" s="21"/>
+      <c r="BL19" s="21"/>
+      <c r="BM19" s="21"/>
+      <c r="BN19" s="21"/>
+      <c r="BO19" s="21"/>
+      <c r="BP19" s="21"/>
+      <c r="BQ19" s="21"/>
+      <c r="BR19" s="21"/>
+      <c r="BS19" s="21"/>
+      <c r="BT19" s="21"/>
+      <c r="BU19" s="21"/>
+      <c r="BV19" s="21"/>
+      <c r="BW19" s="21"/>
+      <c r="BX19" s="21"/>
+      <c r="BY19" s="21"/>
+      <c r="BZ19" s="21"/>
+      <c r="CA19" s="21"/>
+      <c r="CB19" s="21"/>
+      <c r="CC19" s="21"/>
+      <c r="CD19" s="21"/>
+      <c r="CE19" s="21"/>
+      <c r="CF19" s="21"/>
+      <c r="CG19" s="21"/>
+      <c r="CH19" s="21"/>
+      <c r="CI19" s="21"/>
+      <c r="CJ19" s="21"/>
+      <c r="CK19" s="21"/>
+      <c r="CL19" s="21"/>
+      <c r="CM19" s="21"/>
+      <c r="CN19" s="21"/>
+      <c r="CO19" s="21"/>
+      <c r="CP19" s="21"/>
+      <c r="CQ19" s="21"/>
+      <c r="CR19" s="21"/>
+      <c r="CS19" s="21"/>
+      <c r="CT19" s="21"/>
+      <c r="CU19" s="21"/>
+      <c r="CV19" s="21"/>
+      <c r="CW19" s="21"/>
+      <c r="CX19" s="21"/>
+      <c r="CY19" s="21"/>
+      <c r="CZ19" s="21"/>
+      <c r="DA19" s="21"/>
+      <c r="DB19" s="21"/>
+      <c r="DC19" s="21"/>
+      <c r="DD19" s="21"/>
+      <c r="DE19" s="21"/>
+      <c r="DF19" s="21"/>
+      <c r="DG19" s="21"/>
+      <c r="DH19" s="21"/>
+      <c r="DI19" s="21"/>
+      <c r="DJ19" s="21"/>
+      <c r="DK19" s="21"/>
+      <c r="DL19" s="21"/>
+      <c r="DM19" s="21"/>
+    </row>
+    <row r="20" spans="1:117">
       <c r="A20" s="6" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="B20" s="5">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C20" s="47"/>
       <c r="D20" s="47"/>
       <c r="E20" s="54"/>
       <c r="F20" s="47"/>
-      <c r="G20" s="47"/>
+      <c r="G20" s="46"/>
       <c r="H20" s="47"/>
       <c r="I20" s="47"/>
       <c r="J20" s="47"/>
-      <c r="K20" s="52"/>
-      <c r="L20" s="51"/>
+      <c r="K20" s="19"/>
+      <c r="L20" s="17"/>
       <c r="M20" s="47"/>
-      <c r="N20" s="47"/>
+      <c r="N20" s="46"/>
       <c r="O20" s="47"/>
-      <c r="P20" s="51"/>
-      <c r="Q20" s="31"/>
+      <c r="P20" s="17"/>
+      <c r="Q20" s="18"/>
       <c r="R20" s="18"/>
       <c r="S20" s="18"/>
-      <c r="T20" s="27"/>
-      <c r="U20" s="27"/>
-      <c r="V20" s="27"/>
-      <c r="W20" s="27"/>
-      <c r="X20" s="28"/>
-      <c r="Y20" s="21"/>
-      <c r="Z20" s="21"/>
-      <c r="AA20" s="21"/>
-      <c r="AB20" s="21"/>
-      <c r="AC20" s="21"/>
-      <c r="AD20" s="21"/>
-      <c r="AE20" s="21"/>
-      <c r="AF20" s="21"/>
-      <c r="AG20" s="21"/>
-      <c r="AH20" s="21"/>
-      <c r="AI20" s="21"/>
-      <c r="AJ20" s="21"/>
-      <c r="AK20" s="21"/>
-      <c r="AL20" s="21"/>
-      <c r="AM20" s="21"/>
-      <c r="AN20" s="21"/>
-      <c r="AO20" s="21"/>
-      <c r="AP20" s="21"/>
-      <c r="AQ20" s="21"/>
-      <c r="AR20" s="21"/>
-      <c r="AS20" s="21"/>
-      <c r="AT20" s="21"/>
-      <c r="AU20" s="21"/>
-      <c r="AV20" s="21"/>
-      <c r="AW20" s="21"/>
-      <c r="AX20" s="21"/>
-      <c r="AY20" s="21"/>
-      <c r="AZ20" s="21"/>
-      <c r="BA20" s="21"/>
-      <c r="BB20" s="21"/>
-      <c r="BC20" s="21"/>
-      <c r="BD20" s="21"/>
-      <c r="BE20" s="21"/>
-      <c r="BF20" s="21"/>
-      <c r="BG20" s="21"/>
-      <c r="BH20" s="21"/>
-      <c r="BI20" s="21"/>
-      <c r="BJ20" s="21"/>
-      <c r="BK20" s="21"/>
-      <c r="BL20" s="21"/>
-      <c r="BM20" s="21"/>
-      <c r="BN20" s="21"/>
-      <c r="BO20" s="21"/>
-      <c r="BP20" s="21"/>
-      <c r="BQ20" s="21"/>
-      <c r="BR20" s="21"/>
-      <c r="BS20" s="21"/>
-      <c r="BT20" s="21"/>
-      <c r="BU20" s="21"/>
-      <c r="BV20" s="21"/>
-      <c r="BW20" s="21"/>
-      <c r="BX20" s="21"/>
-      <c r="BY20" s="21"/>
-      <c r="BZ20" s="21"/>
-      <c r="CA20" s="21"/>
-      <c r="CB20" s="21"/>
-      <c r="CC20" s="21"/>
-      <c r="CD20" s="21"/>
-      <c r="CE20" s="21"/>
-      <c r="CF20" s="21"/>
-      <c r="CG20" s="21"/>
-      <c r="CH20" s="21"/>
-      <c r="CI20" s="21"/>
-      <c r="CJ20" s="21"/>
-      <c r="CK20" s="21"/>
-      <c r="CL20" s="21"/>
-      <c r="CM20" s="21"/>
-      <c r="CN20" s="21"/>
-      <c r="CO20" s="21"/>
-      <c r="CP20" s="21"/>
-      <c r="CQ20" s="21"/>
-      <c r="CR20" s="21"/>
-      <c r="CS20" s="21"/>
-      <c r="CT20" s="21"/>
-      <c r="CU20" s="21"/>
-      <c r="CV20" s="21"/>
-      <c r="CW20" s="21"/>
-      <c r="CX20" s="21"/>
-      <c r="CY20" s="21"/>
-      <c r="CZ20" s="21"/>
-      <c r="DA20" s="21"/>
-      <c r="DB20" s="21"/>
-      <c r="DC20" s="21"/>
-      <c r="DD20" s="21"/>
-      <c r="DE20" s="21"/>
-      <c r="DF20" s="21"/>
-      <c r="DG20" s="21"/>
-      <c r="DH20" s="21"/>
-      <c r="DI20" s="21"/>
-      <c r="DJ20" s="21"/>
-      <c r="DK20" s="21"/>
-      <c r="DL20" s="21"/>
-      <c r="DM20" s="21"/>
-    </row>
-    <row r="21" spans="1:117" x14ac:dyDescent="0.2">
+      <c r="T20" s="19"/>
+      <c r="U20" s="19"/>
+      <c r="V20" s="19"/>
+      <c r="W20" s="19"/>
+      <c r="X20" s="20"/>
+      <c r="Y20" s="18"/>
+      <c r="Z20" s="18"/>
+      <c r="AA20" s="18"/>
+      <c r="AB20" s="18"/>
+      <c r="AC20" s="18"/>
+      <c r="AD20" s="18"/>
+      <c r="AE20" s="18"/>
+      <c r="AF20" s="18"/>
+      <c r="AG20" s="18"/>
+      <c r="AH20" s="18"/>
+      <c r="AI20" s="18"/>
+      <c r="AJ20" s="18"/>
+      <c r="AK20" s="18"/>
+      <c r="AL20" s="18"/>
+      <c r="AM20" s="18"/>
+      <c r="AN20" s="18"/>
+      <c r="AO20" s="18"/>
+      <c r="AP20" s="18"/>
+      <c r="AQ20" s="18"/>
+      <c r="AR20" s="18"/>
+      <c r="AS20" s="18"/>
+      <c r="AT20" s="18"/>
+      <c r="AU20" s="18"/>
+      <c r="AV20" s="18"/>
+      <c r="AW20" s="18"/>
+      <c r="AX20" s="18"/>
+      <c r="AY20" s="18"/>
+      <c r="AZ20" s="18"/>
+      <c r="BA20" s="18"/>
+      <c r="BB20" s="18"/>
+      <c r="BC20" s="18"/>
+      <c r="BD20" s="18"/>
+      <c r="BE20" s="18"/>
+      <c r="BF20" s="18"/>
+      <c r="BG20" s="18"/>
+      <c r="BH20" s="18"/>
+      <c r="BI20" s="18"/>
+      <c r="BJ20" s="18"/>
+      <c r="BK20" s="18"/>
+      <c r="BL20" s="18"/>
+      <c r="BM20" s="18"/>
+      <c r="BN20" s="18"/>
+      <c r="BO20" s="18"/>
+      <c r="BP20" s="18"/>
+      <c r="BQ20" s="18"/>
+      <c r="BR20" s="18"/>
+      <c r="BS20" s="18"/>
+      <c r="BT20" s="18"/>
+      <c r="BU20" s="18"/>
+      <c r="BV20" s="18"/>
+      <c r="BW20" s="18"/>
+      <c r="BX20" s="18"/>
+      <c r="BY20" s="18"/>
+      <c r="BZ20" s="18"/>
+      <c r="CA20" s="18"/>
+      <c r="CB20" s="18"/>
+      <c r="CC20" s="18"/>
+      <c r="CD20" s="18"/>
+      <c r="CE20" s="18"/>
+      <c r="CF20" s="18"/>
+      <c r="CG20" s="18"/>
+      <c r="CH20" s="18"/>
+      <c r="CI20" s="18"/>
+      <c r="CJ20" s="18"/>
+      <c r="CK20" s="18"/>
+      <c r="CL20" s="18"/>
+      <c r="CM20" s="18"/>
+      <c r="CN20" s="18"/>
+      <c r="CO20" s="18"/>
+      <c r="CP20" s="18"/>
+      <c r="CQ20" s="18"/>
+      <c r="CR20" s="18"/>
+      <c r="CS20" s="18"/>
+      <c r="CT20" s="18"/>
+      <c r="CU20" s="18"/>
+      <c r="CV20" s="18"/>
+      <c r="CW20" s="18"/>
+      <c r="CX20" s="18"/>
+      <c r="CY20" s="18"/>
+      <c r="CZ20" s="18"/>
+      <c r="DA20" s="18"/>
+      <c r="DB20" s="18"/>
+      <c r="DC20" s="18"/>
+      <c r="DD20" s="18"/>
+      <c r="DE20" s="18"/>
+      <c r="DF20" s="18"/>
+      <c r="DG20" s="18"/>
+      <c r="DH20" s="18"/>
+      <c r="DI20" s="18"/>
+      <c r="DJ20" s="18"/>
+      <c r="DK20" s="18"/>
+      <c r="DL20" s="18"/>
+      <c r="DM20" s="18"/>
+    </row>
+    <row r="21" spans="1:117">
       <c r="A21" s="6" t="s">
-        <v>19</v>
+        <v>4</v>
       </c>
       <c r="B21" s="5">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C21" s="47"/>
       <c r="D21" s="47"/>
-      <c r="E21" s="54"/>
+      <c r="E21" s="53"/>
       <c r="F21" s="47"/>
-      <c r="G21" s="46"/>
+      <c r="G21" s="47"/>
       <c r="H21" s="47"/>
       <c r="I21" s="47"/>
-      <c r="J21" s="47"/>
-      <c r="K21" s="19"/>
-      <c r="L21" s="17"/>
+      <c r="J21" s="46"/>
+      <c r="K21" s="18"/>
+      <c r="L21" s="18"/>
       <c r="M21" s="47"/>
-      <c r="N21" s="46"/>
+      <c r="N21" s="57"/>
       <c r="O21" s="47"/>
-      <c r="P21" s="17"/>
+      <c r="P21" s="18"/>
       <c r="Q21" s="18"/>
       <c r="R21" s="18"/>
       <c r="S21" s="18"/>
-      <c r="T21" s="19"/>
-      <c r="U21" s="19"/>
-      <c r="V21" s="19"/>
-      <c r="W21" s="19"/>
-      <c r="X21" s="20"/>
+      <c r="T21" s="18"/>
+      <c r="U21" s="18"/>
+      <c r="V21" s="18"/>
+      <c r="W21" s="18"/>
+      <c r="X21" s="18"/>
       <c r="Y21" s="18"/>
       <c r="Z21" s="18"/>
       <c r="AA21" s="18"/>
@@ -3862,30 +3853,30 @@
       <c r="DL21" s="18"/>
       <c r="DM21" s="18"/>
     </row>
-    <row r="22" spans="1:117" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:117">
       <c r="A22" s="6" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="B22" s="5">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C22" s="47"/>
       <c r="D22" s="47"/>
-      <c r="E22" s="53"/>
+      <c r="E22" s="54"/>
       <c r="F22" s="47"/>
       <c r="G22" s="47"/>
       <c r="H22" s="47"/>
       <c r="I22" s="47"/>
-      <c r="J22" s="46"/>
+      <c r="J22" s="47"/>
       <c r="K22" s="18"/>
       <c r="L22" s="18"/>
-      <c r="M22" s="47"/>
-      <c r="N22" s="57"/>
+      <c r="M22" s="46"/>
+      <c r="N22" s="47"/>
       <c r="O22" s="47"/>
       <c r="P22" s="18"/>
-      <c r="Q22" s="18"/>
-      <c r="R22" s="18"/>
-      <c r="S22" s="18"/>
+      <c r="Q22" s="32"/>
+      <c r="R22" s="31"/>
+      <c r="S22" s="31"/>
       <c r="T22" s="18"/>
       <c r="U22" s="18"/>
       <c r="V22" s="18"/>
@@ -3985,29 +3976,29 @@
       <c r="DL22" s="18"/>
       <c r="DM22" s="18"/>
     </row>
-    <row r="23" spans="1:117" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:117">
       <c r="A23" s="6" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="B23" s="5">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C23" s="47"/>
       <c r="D23" s="47"/>
       <c r="E23" s="54"/>
-      <c r="F23" s="47"/>
+      <c r="F23" s="46"/>
       <c r="G23" s="47"/>
-      <c r="H23" s="47"/>
-      <c r="I23" s="47"/>
+      <c r="H23" s="46"/>
+      <c r="I23" s="46"/>
       <c r="J23" s="47"/>
       <c r="K23" s="18"/>
       <c r="L23" s="18"/>
       <c r="M23" s="46"/>
-      <c r="N23" s="47"/>
-      <c r="O23" s="47"/>
+      <c r="N23" s="46"/>
+      <c r="O23" s="46"/>
       <c r="P23" s="18"/>
-      <c r="Q23" s="32"/>
-      <c r="R23" s="31"/>
+      <c r="Q23" s="18"/>
+      <c r="R23" s="18"/>
       <c r="S23" s="31"/>
       <c r="T23" s="18"/>
       <c r="U23" s="18"/>
@@ -4108,30 +4099,30 @@
       <c r="DL23" s="18"/>
       <c r="DM23" s="18"/>
     </row>
-    <row r="24" spans="1:117" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:117">
       <c r="A24" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B24" s="5">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C24" s="47"/>
       <c r="D24" s="47"/>
       <c r="E24" s="54"/>
-      <c r="F24" s="46"/>
+      <c r="F24" s="47"/>
       <c r="G24" s="47"/>
       <c r="H24" s="46"/>
       <c r="I24" s="46"/>
       <c r="J24" s="47"/>
       <c r="K24" s="18"/>
-      <c r="L24" s="18"/>
-      <c r="M24" s="46"/>
-      <c r="N24" s="46"/>
+      <c r="L24" s="31"/>
+      <c r="M24" s="47"/>
+      <c r="N24" s="47"/>
       <c r="O24" s="46"/>
       <c r="P24" s="18"/>
-      <c r="Q24" s="18"/>
-      <c r="R24" s="18"/>
-      <c r="S24" s="31"/>
+      <c r="Q24" s="32"/>
+      <c r="R24" s="31"/>
+      <c r="S24" s="18"/>
       <c r="T24" s="18"/>
       <c r="U24" s="18"/>
       <c r="V24" s="18"/>
@@ -4231,26 +4222,26 @@
       <c r="DL24" s="18"/>
       <c r="DM24" s="18"/>
     </row>
-    <row r="25" spans="1:117" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:117">
       <c r="A25" s="6" t="s">
-        <v>21</v>
+        <v>5</v>
       </c>
       <c r="B25" s="5">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C25" s="47"/>
       <c r="D25" s="47"/>
       <c r="E25" s="54"/>
       <c r="F25" s="47"/>
       <c r="G25" s="47"/>
-      <c r="H25" s="46"/>
-      <c r="I25" s="46"/>
+      <c r="H25" s="47"/>
+      <c r="I25" s="47"/>
       <c r="J25" s="47"/>
       <c r="K25" s="18"/>
-      <c r="L25" s="31"/>
+      <c r="L25" s="18"/>
       <c r="M25" s="47"/>
       <c r="N25" s="47"/>
-      <c r="O25" s="46"/>
+      <c r="O25" s="47"/>
       <c r="P25" s="18"/>
       <c r="Q25" s="32"/>
       <c r="R25" s="31"/>
@@ -4354,12 +4345,12 @@
       <c r="DL25" s="18"/>
       <c r="DM25" s="18"/>
     </row>
-    <row r="26" spans="1:117" x14ac:dyDescent="0.2">
-      <c r="A26" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="B26" s="5">
-        <v>25</v>
+    <row r="26" spans="1:117" s="12" customFormat="1">
+      <c r="A26" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B26" s="11">
+        <v>26</v>
       </c>
       <c r="C26" s="47"/>
       <c r="D26" s="47"/>
@@ -4368,16 +4359,16 @@
       <c r="G26" s="47"/>
       <c r="H26" s="47"/>
       <c r="I26" s="47"/>
-      <c r="J26" s="47"/>
+      <c r="J26" s="46"/>
       <c r="K26" s="18"/>
-      <c r="L26" s="18"/>
+      <c r="L26" s="31"/>
       <c r="M26" s="47"/>
       <c r="N26" s="47"/>
       <c r="O26" s="47"/>
-      <c r="P26" s="18"/>
-      <c r="Q26" s="32"/>
-      <c r="R26" s="31"/>
-      <c r="S26" s="18"/>
+      <c r="P26" s="31"/>
+      <c r="Q26" s="18"/>
+      <c r="R26" s="18"/>
+      <c r="S26" s="32"/>
       <c r="T26" s="18"/>
       <c r="U26" s="18"/>
       <c r="V26" s="18"/>
@@ -4477,12 +4468,12 @@
       <c r="DL26" s="18"/>
       <c r="DM26" s="18"/>
     </row>
-    <row r="27" spans="1:117" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:117" s="12" customFormat="1" ht="12" thickBot="1">
       <c r="A27" s="10" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="B27" s="11">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C27" s="47"/>
       <c r="D27" s="47"/>
@@ -4493,7 +4484,7 @@
       <c r="I27" s="47"/>
       <c r="J27" s="46"/>
       <c r="K27" s="18"/>
-      <c r="L27" s="31"/>
+      <c r="L27" s="18"/>
       <c r="M27" s="47"/>
       <c r="N27" s="47"/>
       <c r="O27" s="47"/>
@@ -4501,375 +4492,375 @@
       <c r="Q27" s="18"/>
       <c r="R27" s="18"/>
       <c r="S27" s="32"/>
-      <c r="T27" s="18"/>
-      <c r="U27" s="18"/>
-      <c r="V27" s="18"/>
-      <c r="W27" s="18"/>
-      <c r="X27" s="18"/>
-      <c r="Y27" s="18"/>
-      <c r="Z27" s="18"/>
-      <c r="AA27" s="18"/>
-      <c r="AB27" s="18"/>
-      <c r="AC27" s="18"/>
-      <c r="AD27" s="18"/>
-      <c r="AE27" s="18"/>
-      <c r="AF27" s="18"/>
-      <c r="AG27" s="18"/>
-      <c r="AH27" s="18"/>
-      <c r="AI27" s="18"/>
-      <c r="AJ27" s="18"/>
-      <c r="AK27" s="18"/>
-      <c r="AL27" s="18"/>
-      <c r="AM27" s="18"/>
-      <c r="AN27" s="18"/>
-      <c r="AO27" s="18"/>
-      <c r="AP27" s="18"/>
-      <c r="AQ27" s="18"/>
-      <c r="AR27" s="18"/>
-      <c r="AS27" s="18"/>
-      <c r="AT27" s="18"/>
-      <c r="AU27" s="18"/>
-      <c r="AV27" s="18"/>
-      <c r="AW27" s="18"/>
-      <c r="AX27" s="18"/>
-      <c r="AY27" s="18"/>
-      <c r="AZ27" s="18"/>
-      <c r="BA27" s="18"/>
-      <c r="BB27" s="18"/>
-      <c r="BC27" s="18"/>
-      <c r="BD27" s="18"/>
-      <c r="BE27" s="18"/>
-      <c r="BF27" s="18"/>
-      <c r="BG27" s="18"/>
-      <c r="BH27" s="18"/>
-      <c r="BI27" s="18"/>
-      <c r="BJ27" s="18"/>
-      <c r="BK27" s="18"/>
-      <c r="BL27" s="18"/>
-      <c r="BM27" s="18"/>
-      <c r="BN27" s="18"/>
-      <c r="BO27" s="18"/>
-      <c r="BP27" s="18"/>
-      <c r="BQ27" s="18"/>
-      <c r="BR27" s="18"/>
-      <c r="BS27" s="18"/>
-      <c r="BT27" s="18"/>
-      <c r="BU27" s="18"/>
-      <c r="BV27" s="18"/>
-      <c r="BW27" s="18"/>
-      <c r="BX27" s="18"/>
-      <c r="BY27" s="18"/>
-      <c r="BZ27" s="18"/>
-      <c r="CA27" s="18"/>
-      <c r="CB27" s="18"/>
-      <c r="CC27" s="18"/>
-      <c r="CD27" s="18"/>
-      <c r="CE27" s="18"/>
-      <c r="CF27" s="18"/>
-      <c r="CG27" s="18"/>
-      <c r="CH27" s="18"/>
-      <c r="CI27" s="18"/>
-      <c r="CJ27" s="18"/>
-      <c r="CK27" s="18"/>
-      <c r="CL27" s="18"/>
-      <c r="CM27" s="18"/>
-      <c r="CN27" s="18"/>
-      <c r="CO27" s="18"/>
-      <c r="CP27" s="18"/>
-      <c r="CQ27" s="18"/>
-      <c r="CR27" s="18"/>
-      <c r="CS27" s="18"/>
-      <c r="CT27" s="18"/>
-      <c r="CU27" s="18"/>
-      <c r="CV27" s="18"/>
-      <c r="CW27" s="18"/>
-      <c r="CX27" s="18"/>
-      <c r="CY27" s="18"/>
-      <c r="CZ27" s="18"/>
-      <c r="DA27" s="18"/>
-      <c r="DB27" s="18"/>
-      <c r="DC27" s="18"/>
-      <c r="DD27" s="18"/>
-      <c r="DE27" s="18"/>
-      <c r="DF27" s="18"/>
-      <c r="DG27" s="18"/>
-      <c r="DH27" s="18"/>
-      <c r="DI27" s="18"/>
-      <c r="DJ27" s="18"/>
-      <c r="DK27" s="18"/>
-      <c r="DL27" s="18"/>
-      <c r="DM27" s="18"/>
-    </row>
-    <row r="28" spans="1:117" s="12" customFormat="1" ht="12" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="10" t="s">
+      <c r="T27" s="25"/>
+      <c r="U27" s="25"/>
+      <c r="V27" s="25"/>
+      <c r="W27" s="25"/>
+      <c r="X27" s="25"/>
+      <c r="Y27" s="25"/>
+      <c r="Z27" s="25"/>
+      <c r="AA27" s="25"/>
+      <c r="AB27" s="25"/>
+      <c r="AC27" s="25"/>
+      <c r="AD27" s="25"/>
+      <c r="AE27" s="25"/>
+      <c r="AF27" s="25"/>
+      <c r="AG27" s="25"/>
+      <c r="AH27" s="25"/>
+      <c r="AI27" s="25"/>
+      <c r="AJ27" s="25"/>
+      <c r="AK27" s="25"/>
+      <c r="AL27" s="25"/>
+      <c r="AM27" s="25"/>
+      <c r="AN27" s="25"/>
+      <c r="AO27" s="25"/>
+      <c r="AP27" s="25"/>
+      <c r="AQ27" s="25"/>
+      <c r="AR27" s="25"/>
+      <c r="AS27" s="25"/>
+      <c r="AT27" s="25"/>
+      <c r="AU27" s="25"/>
+      <c r="AV27" s="25"/>
+      <c r="AW27" s="25"/>
+      <c r="AX27" s="25"/>
+      <c r="AY27" s="25"/>
+      <c r="AZ27" s="25"/>
+      <c r="BA27" s="25"/>
+      <c r="BB27" s="25"/>
+      <c r="BC27" s="25"/>
+      <c r="BD27" s="25"/>
+      <c r="BE27" s="25"/>
+      <c r="BF27" s="25"/>
+      <c r="BG27" s="25"/>
+      <c r="BH27" s="25"/>
+      <c r="BI27" s="25"/>
+      <c r="BJ27" s="25"/>
+      <c r="BK27" s="25"/>
+      <c r="BL27" s="25"/>
+      <c r="BM27" s="25"/>
+      <c r="BN27" s="25"/>
+      <c r="BO27" s="25"/>
+      <c r="BP27" s="25"/>
+      <c r="BQ27" s="25"/>
+      <c r="BR27" s="25"/>
+      <c r="BS27" s="25"/>
+      <c r="BT27" s="25"/>
+      <c r="BU27" s="25"/>
+      <c r="BV27" s="25"/>
+      <c r="BW27" s="25"/>
+      <c r="BX27" s="25"/>
+      <c r="BY27" s="25"/>
+      <c r="BZ27" s="25"/>
+      <c r="CA27" s="25"/>
+      <c r="CB27" s="25"/>
+      <c r="CC27" s="25"/>
+      <c r="CD27" s="25"/>
+      <c r="CE27" s="25"/>
+      <c r="CF27" s="25"/>
+      <c r="CG27" s="25"/>
+      <c r="CH27" s="25"/>
+      <c r="CI27" s="25"/>
+      <c r="CJ27" s="25"/>
+      <c r="CK27" s="25"/>
+      <c r="CL27" s="25"/>
+      <c r="CM27" s="25"/>
+      <c r="CN27" s="25"/>
+      <c r="CO27" s="25"/>
+      <c r="CP27" s="25"/>
+      <c r="CQ27" s="25"/>
+      <c r="CR27" s="25"/>
+      <c r="CS27" s="25"/>
+      <c r="CT27" s="25"/>
+      <c r="CU27" s="25"/>
+      <c r="CV27" s="25"/>
+      <c r="CW27" s="25"/>
+      <c r="CX27" s="25"/>
+      <c r="CY27" s="25"/>
+      <c r="CZ27" s="25"/>
+      <c r="DA27" s="25"/>
+      <c r="DB27" s="25"/>
+      <c r="DC27" s="25"/>
+      <c r="DD27" s="25"/>
+      <c r="DE27" s="25"/>
+      <c r="DF27" s="25"/>
+      <c r="DG27" s="25"/>
+      <c r="DH27" s="25"/>
+      <c r="DI27" s="25"/>
+      <c r="DJ27" s="25"/>
+      <c r="DK27" s="25"/>
+      <c r="DL27" s="25"/>
+      <c r="DM27" s="25"/>
+    </row>
+    <row r="28" spans="1:117" s="9" customFormat="1">
+      <c r="A28" s="39" t="s">
+        <v>21</v>
+      </c>
+      <c r="B28" s="40">
+        <v>28</v>
+      </c>
+      <c r="C28" s="49"/>
+      <c r="D28" s="49"/>
+      <c r="E28" s="55"/>
+      <c r="F28" s="48"/>
+      <c r="G28" s="48"/>
+      <c r="H28" s="48"/>
+      <c r="I28" s="48"/>
+      <c r="J28" s="48"/>
+      <c r="K28" s="31"/>
+      <c r="L28" s="31"/>
+      <c r="M28" s="48"/>
+      <c r="N28" s="48"/>
+      <c r="O28" s="48"/>
+      <c r="P28" s="31"/>
+      <c r="Q28" s="35"/>
+      <c r="R28" s="35"/>
+      <c r="S28" s="31"/>
+      <c r="T28" s="23"/>
+      <c r="U28" s="23"/>
+      <c r="V28" s="23"/>
+      <c r="W28" s="23"/>
+      <c r="X28" s="23"/>
+      <c r="Y28" s="23"/>
+      <c r="Z28" s="23"/>
+      <c r="AA28" s="23"/>
+      <c r="AB28" s="23"/>
+      <c r="AC28" s="23"/>
+      <c r="AD28" s="23"/>
+      <c r="AE28" s="23"/>
+      <c r="AF28" s="23"/>
+      <c r="AG28" s="23"/>
+      <c r="AH28" s="23"/>
+      <c r="AI28" s="23"/>
+      <c r="AJ28" s="23"/>
+      <c r="AK28" s="23"/>
+      <c r="AL28" s="23"/>
+      <c r="AM28" s="23"/>
+      <c r="AN28" s="23"/>
+      <c r="AO28" s="23"/>
+      <c r="AP28" s="23"/>
+      <c r="AQ28" s="23"/>
+      <c r="AR28" s="23"/>
+      <c r="AS28" s="23"/>
+      <c r="AT28" s="23"/>
+      <c r="AU28" s="23"/>
+      <c r="AV28" s="23"/>
+      <c r="AW28" s="23"/>
+      <c r="AX28" s="23"/>
+      <c r="AY28" s="23"/>
+      <c r="AZ28" s="23"/>
+      <c r="BA28" s="23"/>
+      <c r="BB28" s="23"/>
+      <c r="BC28" s="23"/>
+      <c r="BD28" s="23"/>
+      <c r="BE28" s="23"/>
+      <c r="BF28" s="23"/>
+      <c r="BG28" s="23"/>
+      <c r="BH28" s="23"/>
+      <c r="BI28" s="23"/>
+      <c r="BJ28" s="23"/>
+      <c r="BK28" s="23"/>
+      <c r="BL28" s="23"/>
+      <c r="BM28" s="23"/>
+      <c r="BN28" s="23"/>
+      <c r="BO28" s="23"/>
+      <c r="BP28" s="23"/>
+      <c r="BQ28" s="23"/>
+      <c r="BR28" s="23"/>
+      <c r="BS28" s="23"/>
+      <c r="BT28" s="23"/>
+      <c r="BU28" s="23"/>
+      <c r="BV28" s="23"/>
+      <c r="BW28" s="23"/>
+      <c r="BX28" s="23"/>
+      <c r="BY28" s="23"/>
+      <c r="BZ28" s="23"/>
+      <c r="CA28" s="23"/>
+      <c r="CB28" s="23"/>
+      <c r="CC28" s="23"/>
+      <c r="CD28" s="23"/>
+      <c r="CE28" s="23"/>
+      <c r="CF28" s="23"/>
+      <c r="CG28" s="23"/>
+      <c r="CH28" s="23"/>
+      <c r="CI28" s="23"/>
+      <c r="CJ28" s="23"/>
+      <c r="CK28" s="23"/>
+      <c r="CL28" s="23"/>
+      <c r="CM28" s="23"/>
+      <c r="CN28" s="23"/>
+      <c r="CO28" s="23"/>
+      <c r="CP28" s="23"/>
+      <c r="CQ28" s="23"/>
+      <c r="CR28" s="23"/>
+      <c r="CS28" s="23"/>
+      <c r="CT28" s="23"/>
+      <c r="CU28" s="23"/>
+      <c r="CV28" s="23"/>
+      <c r="CW28" s="23"/>
+      <c r="CX28" s="23"/>
+      <c r="CY28" s="23"/>
+      <c r="CZ28" s="23"/>
+      <c r="DA28" s="23"/>
+      <c r="DB28" s="23"/>
+      <c r="DC28" s="23"/>
+      <c r="DD28" s="23"/>
+      <c r="DE28" s="23"/>
+      <c r="DF28" s="23"/>
+      <c r="DG28" s="23"/>
+      <c r="DH28" s="23"/>
+      <c r="DI28" s="23"/>
+      <c r="DJ28" s="23"/>
+      <c r="DK28" s="23"/>
+      <c r="DL28" s="23"/>
+      <c r="DM28" s="23"/>
+    </row>
+    <row r="29" spans="1:117" s="12" customFormat="1">
+      <c r="A29" s="41" t="s">
         <v>22</v>
       </c>
-      <c r="B28" s="11">
-        <v>27</v>
-      </c>
-      <c r="C28" s="47"/>
-      <c r="D28" s="47"/>
-      <c r="E28" s="54"/>
-      <c r="F28" s="47"/>
-      <c r="G28" s="47"/>
-      <c r="H28" s="47"/>
-      <c r="I28" s="47"/>
-      <c r="J28" s="46"/>
-      <c r="K28" s="18"/>
-      <c r="L28" s="18"/>
-      <c r="M28" s="47"/>
-      <c r="N28" s="47"/>
-      <c r="O28" s="47"/>
-      <c r="P28" s="31"/>
-      <c r="Q28" s="18"/>
-      <c r="R28" s="18"/>
-      <c r="S28" s="32"/>
-      <c r="T28" s="25"/>
-      <c r="U28" s="25"/>
-      <c r="V28" s="25"/>
-      <c r="W28" s="25"/>
-      <c r="X28" s="25"/>
-      <c r="Y28" s="25"/>
-      <c r="Z28" s="25"/>
-      <c r="AA28" s="25"/>
-      <c r="AB28" s="25"/>
-      <c r="AC28" s="25"/>
-      <c r="AD28" s="25"/>
-      <c r="AE28" s="25"/>
-      <c r="AF28" s="25"/>
-      <c r="AG28" s="25"/>
-      <c r="AH28" s="25"/>
-      <c r="AI28" s="25"/>
-      <c r="AJ28" s="25"/>
-      <c r="AK28" s="25"/>
-      <c r="AL28" s="25"/>
-      <c r="AM28" s="25"/>
-      <c r="AN28" s="25"/>
-      <c r="AO28" s="25"/>
-      <c r="AP28" s="25"/>
-      <c r="AQ28" s="25"/>
-      <c r="AR28" s="25"/>
-      <c r="AS28" s="25"/>
-      <c r="AT28" s="25"/>
-      <c r="AU28" s="25"/>
-      <c r="AV28" s="25"/>
-      <c r="AW28" s="25"/>
-      <c r="AX28" s="25"/>
-      <c r="AY28" s="25"/>
-      <c r="AZ28" s="25"/>
-      <c r="BA28" s="25"/>
-      <c r="BB28" s="25"/>
-      <c r="BC28" s="25"/>
-      <c r="BD28" s="25"/>
-      <c r="BE28" s="25"/>
-      <c r="BF28" s="25"/>
-      <c r="BG28" s="25"/>
-      <c r="BH28" s="25"/>
-      <c r="BI28" s="25"/>
-      <c r="BJ28" s="25"/>
-      <c r="BK28" s="25"/>
-      <c r="BL28" s="25"/>
-      <c r="BM28" s="25"/>
-      <c r="BN28" s="25"/>
-      <c r="BO28" s="25"/>
-      <c r="BP28" s="25"/>
-      <c r="BQ28" s="25"/>
-      <c r="BR28" s="25"/>
-      <c r="BS28" s="25"/>
-      <c r="BT28" s="25"/>
-      <c r="BU28" s="25"/>
-      <c r="BV28" s="25"/>
-      <c r="BW28" s="25"/>
-      <c r="BX28" s="25"/>
-      <c r="BY28" s="25"/>
-      <c r="BZ28" s="25"/>
-      <c r="CA28" s="25"/>
-      <c r="CB28" s="25"/>
-      <c r="CC28" s="25"/>
-      <c r="CD28" s="25"/>
-      <c r="CE28" s="25"/>
-      <c r="CF28" s="25"/>
-      <c r="CG28" s="25"/>
-      <c r="CH28" s="25"/>
-      <c r="CI28" s="25"/>
-      <c r="CJ28" s="25"/>
-      <c r="CK28" s="25"/>
-      <c r="CL28" s="25"/>
-      <c r="CM28" s="25"/>
-      <c r="CN28" s="25"/>
-      <c r="CO28" s="25"/>
-      <c r="CP28" s="25"/>
-      <c r="CQ28" s="25"/>
-      <c r="CR28" s="25"/>
-      <c r="CS28" s="25"/>
-      <c r="CT28" s="25"/>
-      <c r="CU28" s="25"/>
-      <c r="CV28" s="25"/>
-      <c r="CW28" s="25"/>
-      <c r="CX28" s="25"/>
-      <c r="CY28" s="25"/>
-      <c r="CZ28" s="25"/>
-      <c r="DA28" s="25"/>
-      <c r="DB28" s="25"/>
-      <c r="DC28" s="25"/>
-      <c r="DD28" s="25"/>
-      <c r="DE28" s="25"/>
-      <c r="DF28" s="25"/>
-      <c r="DG28" s="25"/>
-      <c r="DH28" s="25"/>
-      <c r="DI28" s="25"/>
-      <c r="DJ28" s="25"/>
-      <c r="DK28" s="25"/>
-      <c r="DL28" s="25"/>
-      <c r="DM28" s="25"/>
-    </row>
-    <row r="29" spans="1:117" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="39" t="s">
-        <v>23</v>
-      </c>
-      <c r="B29" s="40">
-        <v>28</v>
+      <c r="B29" s="42">
+        <v>29</v>
       </c>
       <c r="C29" s="49"/>
       <c r="D29" s="49"/>
       <c r="E29" s="55"/>
-      <c r="F29" s="48"/>
-      <c r="G29" s="48"/>
-      <c r="H29" s="48"/>
-      <c r="I29" s="48"/>
-      <c r="J29" s="48"/>
-      <c r="K29" s="31"/>
-      <c r="L29" s="31"/>
-      <c r="M29" s="48"/>
-      <c r="N29" s="48"/>
-      <c r="O29" s="48"/>
-      <c r="P29" s="31"/>
-      <c r="Q29" s="35"/>
-      <c r="R29" s="35"/>
-      <c r="S29" s="31"/>
-      <c r="T29" s="23"/>
-      <c r="U29" s="23"/>
-      <c r="V29" s="23"/>
-      <c r="W29" s="23"/>
-      <c r="X29" s="23"/>
-      <c r="Y29" s="23"/>
-      <c r="Z29" s="23"/>
-      <c r="AA29" s="23"/>
-      <c r="AB29" s="23"/>
-      <c r="AC29" s="23"/>
-      <c r="AD29" s="23"/>
-      <c r="AE29" s="23"/>
-      <c r="AF29" s="23"/>
-      <c r="AG29" s="23"/>
-      <c r="AH29" s="23"/>
-      <c r="AI29" s="23"/>
-      <c r="AJ29" s="23"/>
-      <c r="AK29" s="23"/>
-      <c r="AL29" s="23"/>
-      <c r="AM29" s="23"/>
-      <c r="AN29" s="23"/>
-      <c r="AO29" s="23"/>
-      <c r="AP29" s="23"/>
-      <c r="AQ29" s="23"/>
-      <c r="AR29" s="23"/>
-      <c r="AS29" s="23"/>
-      <c r="AT29" s="23"/>
-      <c r="AU29" s="23"/>
-      <c r="AV29" s="23"/>
-      <c r="AW29" s="23"/>
-      <c r="AX29" s="23"/>
-      <c r="AY29" s="23"/>
-      <c r="AZ29" s="23"/>
-      <c r="BA29" s="23"/>
-      <c r="BB29" s="23"/>
-      <c r="BC29" s="23"/>
-      <c r="BD29" s="23"/>
-      <c r="BE29" s="23"/>
-      <c r="BF29" s="23"/>
-      <c r="BG29" s="23"/>
-      <c r="BH29" s="23"/>
-      <c r="BI29" s="23"/>
-      <c r="BJ29" s="23"/>
-      <c r="BK29" s="23"/>
-      <c r="BL29" s="23"/>
-      <c r="BM29" s="23"/>
-      <c r="BN29" s="23"/>
-      <c r="BO29" s="23"/>
-      <c r="BP29" s="23"/>
-      <c r="BQ29" s="23"/>
-      <c r="BR29" s="23"/>
-      <c r="BS29" s="23"/>
-      <c r="BT29" s="23"/>
-      <c r="BU29" s="23"/>
-      <c r="BV29" s="23"/>
-      <c r="BW29" s="23"/>
-      <c r="BX29" s="23"/>
-      <c r="BY29" s="23"/>
-      <c r="BZ29" s="23"/>
-      <c r="CA29" s="23"/>
-      <c r="CB29" s="23"/>
-      <c r="CC29" s="23"/>
-      <c r="CD29" s="23"/>
-      <c r="CE29" s="23"/>
-      <c r="CF29" s="23"/>
-      <c r="CG29" s="23"/>
-      <c r="CH29" s="23"/>
-      <c r="CI29" s="23"/>
-      <c r="CJ29" s="23"/>
-      <c r="CK29" s="23"/>
-      <c r="CL29" s="23"/>
-      <c r="CM29" s="23"/>
-      <c r="CN29" s="23"/>
-      <c r="CO29" s="23"/>
-      <c r="CP29" s="23"/>
-      <c r="CQ29" s="23"/>
-      <c r="CR29" s="23"/>
-      <c r="CS29" s="23"/>
-      <c r="CT29" s="23"/>
-      <c r="CU29" s="23"/>
-      <c r="CV29" s="23"/>
-      <c r="CW29" s="23"/>
-      <c r="CX29" s="23"/>
-      <c r="CY29" s="23"/>
-      <c r="CZ29" s="23"/>
-      <c r="DA29" s="23"/>
-      <c r="DB29" s="23"/>
-      <c r="DC29" s="23"/>
-      <c r="DD29" s="23"/>
-      <c r="DE29" s="23"/>
-      <c r="DF29" s="23"/>
-      <c r="DG29" s="23"/>
-      <c r="DH29" s="23"/>
-      <c r="DI29" s="23"/>
-      <c r="DJ29" s="23"/>
-      <c r="DK29" s="23"/>
-      <c r="DL29" s="23"/>
-      <c r="DM29" s="23"/>
-    </row>
-    <row r="30" spans="1:117" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="F29" s="49"/>
+      <c r="G29" s="49"/>
+      <c r="H29" s="49"/>
+      <c r="I29" s="49"/>
+      <c r="J29" s="49"/>
+      <c r="K29" s="18"/>
+      <c r="L29" s="18"/>
+      <c r="M29" s="49"/>
+      <c r="N29" s="49"/>
+      <c r="O29" s="49"/>
+      <c r="P29" s="18"/>
+      <c r="Q29" s="34"/>
+      <c r="R29" s="34"/>
+      <c r="S29" s="18"/>
+      <c r="T29" s="18"/>
+      <c r="U29" s="18"/>
+      <c r="V29" s="18"/>
+      <c r="W29" s="18"/>
+      <c r="X29" s="18"/>
+      <c r="Y29" s="18"/>
+      <c r="Z29" s="18"/>
+      <c r="AA29" s="18"/>
+      <c r="AB29" s="18"/>
+      <c r="AC29" s="18"/>
+      <c r="AD29" s="18"/>
+      <c r="AE29" s="18"/>
+      <c r="AF29" s="18"/>
+      <c r="AG29" s="18"/>
+      <c r="AH29" s="18"/>
+      <c r="AI29" s="18"/>
+      <c r="AJ29" s="18"/>
+      <c r="AK29" s="18"/>
+      <c r="AL29" s="18"/>
+      <c r="AM29" s="18"/>
+      <c r="AN29" s="18"/>
+      <c r="AO29" s="18"/>
+      <c r="AP29" s="18"/>
+      <c r="AQ29" s="18"/>
+      <c r="AR29" s="18"/>
+      <c r="AS29" s="18"/>
+      <c r="AT29" s="18"/>
+      <c r="AU29" s="18"/>
+      <c r="AV29" s="18"/>
+      <c r="AW29" s="18"/>
+      <c r="AX29" s="18"/>
+      <c r="AY29" s="18"/>
+      <c r="AZ29" s="18"/>
+      <c r="BA29" s="18"/>
+      <c r="BB29" s="18"/>
+      <c r="BC29" s="18"/>
+      <c r="BD29" s="18"/>
+      <c r="BE29" s="18"/>
+      <c r="BF29" s="18"/>
+      <c r="BG29" s="18"/>
+      <c r="BH29" s="18"/>
+      <c r="BI29" s="18"/>
+      <c r="BJ29" s="18"/>
+      <c r="BK29" s="18"/>
+      <c r="BL29" s="18"/>
+      <c r="BM29" s="18"/>
+      <c r="BN29" s="18"/>
+      <c r="BO29" s="18"/>
+      <c r="BP29" s="18"/>
+      <c r="BQ29" s="18"/>
+      <c r="BR29" s="18"/>
+      <c r="BS29" s="18"/>
+      <c r="BT29" s="18"/>
+      <c r="BU29" s="18"/>
+      <c r="BV29" s="18"/>
+      <c r="BW29" s="18"/>
+      <c r="BX29" s="18"/>
+      <c r="BY29" s="18"/>
+      <c r="BZ29" s="18"/>
+      <c r="CA29" s="18"/>
+      <c r="CB29" s="18"/>
+      <c r="CC29" s="18"/>
+      <c r="CD29" s="18"/>
+      <c r="CE29" s="18"/>
+      <c r="CF29" s="18"/>
+      <c r="CG29" s="18"/>
+      <c r="CH29" s="18"/>
+      <c r="CI29" s="18"/>
+      <c r="CJ29" s="18"/>
+      <c r="CK29" s="18"/>
+      <c r="CL29" s="18"/>
+      <c r="CM29" s="18"/>
+      <c r="CN29" s="18"/>
+      <c r="CO29" s="18"/>
+      <c r="CP29" s="18"/>
+      <c r="CQ29" s="18"/>
+      <c r="CR29" s="18"/>
+      <c r="CS29" s="18"/>
+      <c r="CT29" s="18"/>
+      <c r="CU29" s="18"/>
+      <c r="CV29" s="18"/>
+      <c r="CW29" s="18"/>
+      <c r="CX29" s="18"/>
+      <c r="CY29" s="18"/>
+      <c r="CZ29" s="18"/>
+      <c r="DA29" s="18"/>
+      <c r="DB29" s="18"/>
+      <c r="DC29" s="18"/>
+      <c r="DD29" s="18"/>
+      <c r="DE29" s="18"/>
+      <c r="DF29" s="18"/>
+      <c r="DG29" s="18"/>
+      <c r="DH29" s="18"/>
+      <c r="DI29" s="18"/>
+      <c r="DJ29" s="18"/>
+      <c r="DK29" s="18"/>
+      <c r="DL29" s="18"/>
+      <c r="DM29" s="18"/>
+    </row>
+    <row r="30" spans="1:117" s="12" customFormat="1">
       <c r="A30" s="41" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B30" s="42">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C30" s="49"/>
       <c r="D30" s="49"/>
       <c r="E30" s="55"/>
       <c r="F30" s="49"/>
-      <c r="G30" s="49"/>
-      <c r="H30" s="49"/>
-      <c r="I30" s="49"/>
-      <c r="J30" s="49"/>
-      <c r="K30" s="18"/>
-      <c r="L30" s="18"/>
-      <c r="M30" s="49"/>
-      <c r="N30" s="49"/>
-      <c r="O30" s="49"/>
-      <c r="P30" s="18"/>
-      <c r="Q30" s="34"/>
-      <c r="R30" s="34"/>
-      <c r="S30" s="18"/>
+      <c r="G30" s="48"/>
+      <c r="H30" s="48"/>
+      <c r="I30" s="48"/>
+      <c r="J30" s="48"/>
+      <c r="K30" s="31"/>
+      <c r="L30" s="31"/>
+      <c r="M30" s="48"/>
+      <c r="N30" s="48"/>
+      <c r="O30" s="48"/>
+      <c r="P30" s="31"/>
+      <c r="Q30" s="35"/>
+      <c r="R30" s="35"/>
+      <c r="S30" s="31"/>
       <c r="T30" s="18"/>
       <c r="U30" s="18"/>
       <c r="V30" s="18"/>
@@ -4969,12 +4960,12 @@
       <c r="DL30" s="18"/>
       <c r="DM30" s="18"/>
     </row>
-    <row r="31" spans="1:117" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:117" s="12" customFormat="1">
       <c r="A31" s="41" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B31" s="42">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C31" s="49"/>
       <c r="D31" s="49"/>
@@ -4983,13 +4974,13 @@
       <c r="G31" s="48"/>
       <c r="H31" s="48"/>
       <c r="I31" s="48"/>
-      <c r="J31" s="48"/>
-      <c r="K31" s="31"/>
-      <c r="L31" s="31"/>
+      <c r="J31" s="49"/>
+      <c r="K31" s="18"/>
+      <c r="L31" s="18"/>
       <c r="M31" s="48"/>
       <c r="N31" s="48"/>
       <c r="O31" s="48"/>
-      <c r="P31" s="31"/>
+      <c r="P31" s="18"/>
       <c r="Q31" s="35"/>
       <c r="R31" s="35"/>
       <c r="S31" s="31"/>
@@ -5092,12 +5083,12 @@
       <c r="DL31" s="18"/>
       <c r="DM31" s="18"/>
     </row>
-    <row r="32" spans="1:117" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:117" s="12" customFormat="1">
       <c r="A32" s="41" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B32" s="42">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C32" s="49"/>
       <c r="D32" s="49"/>
@@ -5105,16 +5096,16 @@
       <c r="F32" s="49"/>
       <c r="G32" s="48"/>
       <c r="H32" s="48"/>
-      <c r="I32" s="48"/>
+      <c r="I32" s="49"/>
       <c r="J32" s="49"/>
       <c r="K32" s="18"/>
       <c r="L32" s="18"/>
-      <c r="M32" s="48"/>
+      <c r="M32" s="49"/>
       <c r="N32" s="48"/>
-      <c r="O32" s="48"/>
+      <c r="O32" s="49"/>
       <c r="P32" s="18"/>
       <c r="Q32" s="35"/>
-      <c r="R32" s="35"/>
+      <c r="R32" s="36"/>
       <c r="S32" s="31"/>
       <c r="T32" s="18"/>
       <c r="U32" s="18"/>
@@ -5215,12 +5206,12 @@
       <c r="DL32" s="18"/>
       <c r="DM32" s="18"/>
     </row>
-    <row r="33" spans="1:117" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="41" t="s">
-        <v>27</v>
-      </c>
-      <c r="B33" s="42">
-        <v>32</v>
+    <row r="33" spans="1:117" s="15" customFormat="1" ht="12" thickBot="1">
+      <c r="A33" s="43" t="s">
+        <v>26</v>
+      </c>
+      <c r="B33" s="44">
+        <v>33</v>
       </c>
       <c r="C33" s="49"/>
       <c r="D33" s="49"/>
@@ -5233,124 +5224,124 @@
       <c r="K33" s="18"/>
       <c r="L33" s="18"/>
       <c r="M33" s="49"/>
-      <c r="N33" s="48"/>
+      <c r="N33" s="49"/>
       <c r="O33" s="49"/>
       <c r="P33" s="18"/>
       <c r="Q33" s="35"/>
       <c r="R33" s="36"/>
-      <c r="S33" s="31"/>
-      <c r="T33" s="18"/>
-      <c r="U33" s="18"/>
-      <c r="V33" s="18"/>
-      <c r="W33" s="18"/>
-      <c r="X33" s="18"/>
-      <c r="Y33" s="18"/>
-      <c r="Z33" s="18"/>
-      <c r="AA33" s="18"/>
-      <c r="AB33" s="18"/>
-      <c r="AC33" s="18"/>
-      <c r="AD33" s="18"/>
-      <c r="AE33" s="18"/>
-      <c r="AF33" s="18"/>
-      <c r="AG33" s="18"/>
-      <c r="AH33" s="18"/>
-      <c r="AI33" s="18"/>
-      <c r="AJ33" s="18"/>
-      <c r="AK33" s="18"/>
-      <c r="AL33" s="18"/>
-      <c r="AM33" s="18"/>
-      <c r="AN33" s="18"/>
-      <c r="AO33" s="18"/>
-      <c r="AP33" s="18"/>
-      <c r="AQ33" s="18"/>
-      <c r="AR33" s="18"/>
-      <c r="AS33" s="18"/>
-      <c r="AT33" s="18"/>
-      <c r="AU33" s="18"/>
-      <c r="AV33" s="18"/>
-      <c r="AW33" s="18"/>
-      <c r="AX33" s="18"/>
-      <c r="AY33" s="18"/>
-      <c r="AZ33" s="18"/>
-      <c r="BA33" s="18"/>
-      <c r="BB33" s="18"/>
-      <c r="BC33" s="18"/>
-      <c r="BD33" s="18"/>
-      <c r="BE33" s="18"/>
-      <c r="BF33" s="18"/>
-      <c r="BG33" s="18"/>
-      <c r="BH33" s="18"/>
-      <c r="BI33" s="18"/>
-      <c r="BJ33" s="18"/>
-      <c r="BK33" s="18"/>
-      <c r="BL33" s="18"/>
-      <c r="BM33" s="18"/>
-      <c r="BN33" s="18"/>
-      <c r="BO33" s="18"/>
-      <c r="BP33" s="18"/>
-      <c r="BQ33" s="18"/>
-      <c r="BR33" s="18"/>
-      <c r="BS33" s="18"/>
-      <c r="BT33" s="18"/>
-      <c r="BU33" s="18"/>
-      <c r="BV33" s="18"/>
-      <c r="BW33" s="18"/>
-      <c r="BX33" s="18"/>
-      <c r="BY33" s="18"/>
-      <c r="BZ33" s="18"/>
-      <c r="CA33" s="18"/>
-      <c r="CB33" s="18"/>
-      <c r="CC33" s="18"/>
-      <c r="CD33" s="18"/>
-      <c r="CE33" s="18"/>
-      <c r="CF33" s="18"/>
-      <c r="CG33" s="18"/>
-      <c r="CH33" s="18"/>
-      <c r="CI33" s="18"/>
-      <c r="CJ33" s="18"/>
-      <c r="CK33" s="18"/>
-      <c r="CL33" s="18"/>
-      <c r="CM33" s="18"/>
-      <c r="CN33" s="18"/>
-      <c r="CO33" s="18"/>
-      <c r="CP33" s="18"/>
-      <c r="CQ33" s="18"/>
-      <c r="CR33" s="18"/>
-      <c r="CS33" s="18"/>
-      <c r="CT33" s="18"/>
-      <c r="CU33" s="18"/>
-      <c r="CV33" s="18"/>
-      <c r="CW33" s="18"/>
-      <c r="CX33" s="18"/>
-      <c r="CY33" s="18"/>
-      <c r="CZ33" s="18"/>
-      <c r="DA33" s="18"/>
-      <c r="DB33" s="18"/>
-      <c r="DC33" s="18"/>
-      <c r="DD33" s="18"/>
-      <c r="DE33" s="18"/>
-      <c r="DF33" s="18"/>
-      <c r="DG33" s="18"/>
-      <c r="DH33" s="18"/>
-      <c r="DI33" s="18"/>
-      <c r="DJ33" s="18"/>
-      <c r="DK33" s="18"/>
-      <c r="DL33" s="18"/>
-      <c r="DM33" s="18"/>
-    </row>
-    <row r="34" spans="1:117" s="15" customFormat="1" ht="12" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="43" t="s">
-        <v>28</v>
-      </c>
-      <c r="B34" s="44">
-        <v>33</v>
+      <c r="S33" s="18"/>
+      <c r="T33" s="24"/>
+      <c r="U33" s="24"/>
+      <c r="V33" s="24"/>
+      <c r="W33" s="24"/>
+      <c r="X33" s="24"/>
+      <c r="Y33" s="24"/>
+      <c r="Z33" s="24"/>
+      <c r="AA33" s="24"/>
+      <c r="AB33" s="24"/>
+      <c r="AC33" s="24"/>
+      <c r="AD33" s="24"/>
+      <c r="AE33" s="24"/>
+      <c r="AF33" s="24"/>
+      <c r="AG33" s="24"/>
+      <c r="AH33" s="24"/>
+      <c r="AI33" s="24"/>
+      <c r="AJ33" s="24"/>
+      <c r="AK33" s="24"/>
+      <c r="AL33" s="24"/>
+      <c r="AM33" s="24"/>
+      <c r="AN33" s="24"/>
+      <c r="AO33" s="24"/>
+      <c r="AP33" s="24"/>
+      <c r="AQ33" s="24"/>
+      <c r="AR33" s="24"/>
+      <c r="AS33" s="24"/>
+      <c r="AT33" s="24"/>
+      <c r="AU33" s="24"/>
+      <c r="AV33" s="24"/>
+      <c r="AW33" s="24"/>
+      <c r="AX33" s="24"/>
+      <c r="AY33" s="24"/>
+      <c r="AZ33" s="24"/>
+      <c r="BA33" s="24"/>
+      <c r="BB33" s="24"/>
+      <c r="BC33" s="24"/>
+      <c r="BD33" s="24"/>
+      <c r="BE33" s="24"/>
+      <c r="BF33" s="24"/>
+      <c r="BG33" s="24"/>
+      <c r="BH33" s="24"/>
+      <c r="BI33" s="24"/>
+      <c r="BJ33" s="24"/>
+      <c r="BK33" s="24"/>
+      <c r="BL33" s="24"/>
+      <c r="BM33" s="24"/>
+      <c r="BN33" s="24"/>
+      <c r="BO33" s="24"/>
+      <c r="BP33" s="24"/>
+      <c r="BQ33" s="24"/>
+      <c r="BR33" s="24"/>
+      <c r="BS33" s="24"/>
+      <c r="BT33" s="24"/>
+      <c r="BU33" s="24"/>
+      <c r="BV33" s="24"/>
+      <c r="BW33" s="24"/>
+      <c r="BX33" s="24"/>
+      <c r="BY33" s="24"/>
+      <c r="BZ33" s="24"/>
+      <c r="CA33" s="24"/>
+      <c r="CB33" s="24"/>
+      <c r="CC33" s="24"/>
+      <c r="CD33" s="24"/>
+      <c r="CE33" s="24"/>
+      <c r="CF33" s="24"/>
+      <c r="CG33" s="24"/>
+      <c r="CH33" s="24"/>
+      <c r="CI33" s="24"/>
+      <c r="CJ33" s="24"/>
+      <c r="CK33" s="24"/>
+      <c r="CL33" s="24"/>
+      <c r="CM33" s="24"/>
+      <c r="CN33" s="24"/>
+      <c r="CO33" s="24"/>
+      <c r="CP33" s="24"/>
+      <c r="CQ33" s="24"/>
+      <c r="CR33" s="24"/>
+      <c r="CS33" s="24"/>
+      <c r="CT33" s="24"/>
+      <c r="CU33" s="24"/>
+      <c r="CV33" s="24"/>
+      <c r="CW33" s="24"/>
+      <c r="CX33" s="24"/>
+      <c r="CY33" s="24"/>
+      <c r="CZ33" s="24"/>
+      <c r="DA33" s="24"/>
+      <c r="DB33" s="24"/>
+      <c r="DC33" s="24"/>
+      <c r="DD33" s="24"/>
+      <c r="DE33" s="24"/>
+      <c r="DF33" s="24"/>
+      <c r="DG33" s="24"/>
+      <c r="DH33" s="24"/>
+      <c r="DI33" s="24"/>
+      <c r="DJ33" s="24"/>
+      <c r="DK33" s="24"/>
+      <c r="DL33" s="24"/>
+      <c r="DM33" s="24"/>
+    </row>
+    <row r="34" spans="1:117" s="9" customFormat="1">
+      <c r="A34" s="39" t="s">
+        <v>27</v>
+      </c>
+      <c r="B34" s="40">
+        <v>34</v>
       </c>
       <c r="C34" s="49"/>
       <c r="D34" s="49"/>
-      <c r="E34" s="55"/>
+      <c r="E34" s="56"/>
       <c r="F34" s="49"/>
-      <c r="G34" s="48"/>
-      <c r="H34" s="48"/>
+      <c r="G34" s="49"/>
+      <c r="H34" s="49"/>
       <c r="I34" s="49"/>
       <c r="J34" s="49"/>
       <c r="K34" s="18"/>
@@ -5359,120 +5350,120 @@
       <c r="N34" s="49"/>
       <c r="O34" s="49"/>
       <c r="P34" s="18"/>
-      <c r="Q34" s="35"/>
-      <c r="R34" s="36"/>
+      <c r="Q34" s="18"/>
+      <c r="R34" s="18"/>
       <c r="S34" s="18"/>
-      <c r="T34" s="24"/>
-      <c r="U34" s="24"/>
-      <c r="V34" s="24"/>
-      <c r="W34" s="24"/>
-      <c r="X34" s="24"/>
-      <c r="Y34" s="24"/>
-      <c r="Z34" s="24"/>
-      <c r="AA34" s="24"/>
-      <c r="AB34" s="24"/>
-      <c r="AC34" s="24"/>
-      <c r="AD34" s="24"/>
-      <c r="AE34" s="24"/>
-      <c r="AF34" s="24"/>
-      <c r="AG34" s="24"/>
-      <c r="AH34" s="24"/>
-      <c r="AI34" s="24"/>
-      <c r="AJ34" s="24"/>
-      <c r="AK34" s="24"/>
-      <c r="AL34" s="24"/>
-      <c r="AM34" s="24"/>
-      <c r="AN34" s="24"/>
-      <c r="AO34" s="24"/>
-      <c r="AP34" s="24"/>
-      <c r="AQ34" s="24"/>
-      <c r="AR34" s="24"/>
-      <c r="AS34" s="24"/>
-      <c r="AT34" s="24"/>
-      <c r="AU34" s="24"/>
-      <c r="AV34" s="24"/>
-      <c r="AW34" s="24"/>
-      <c r="AX34" s="24"/>
-      <c r="AY34" s="24"/>
-      <c r="AZ34" s="24"/>
-      <c r="BA34" s="24"/>
-      <c r="BB34" s="24"/>
-      <c r="BC34" s="24"/>
-      <c r="BD34" s="24"/>
-      <c r="BE34" s="24"/>
-      <c r="BF34" s="24"/>
-      <c r="BG34" s="24"/>
-      <c r="BH34" s="24"/>
-      <c r="BI34" s="24"/>
-      <c r="BJ34" s="24"/>
-      <c r="BK34" s="24"/>
-      <c r="BL34" s="24"/>
-      <c r="BM34" s="24"/>
-      <c r="BN34" s="24"/>
-      <c r="BO34" s="24"/>
-      <c r="BP34" s="24"/>
-      <c r="BQ34" s="24"/>
-      <c r="BR34" s="24"/>
-      <c r="BS34" s="24"/>
-      <c r="BT34" s="24"/>
-      <c r="BU34" s="24"/>
-      <c r="BV34" s="24"/>
-      <c r="BW34" s="24"/>
-      <c r="BX34" s="24"/>
-      <c r="BY34" s="24"/>
-      <c r="BZ34" s="24"/>
-      <c r="CA34" s="24"/>
-      <c r="CB34" s="24"/>
-      <c r="CC34" s="24"/>
-      <c r="CD34" s="24"/>
-      <c r="CE34" s="24"/>
-      <c r="CF34" s="24"/>
-      <c r="CG34" s="24"/>
-      <c r="CH34" s="24"/>
-      <c r="CI34" s="24"/>
-      <c r="CJ34" s="24"/>
-      <c r="CK34" s="24"/>
-      <c r="CL34" s="24"/>
-      <c r="CM34" s="24"/>
-      <c r="CN34" s="24"/>
-      <c r="CO34" s="24"/>
-      <c r="CP34" s="24"/>
-      <c r="CQ34" s="24"/>
-      <c r="CR34" s="24"/>
-      <c r="CS34" s="24"/>
-      <c r="CT34" s="24"/>
-      <c r="CU34" s="24"/>
-      <c r="CV34" s="24"/>
-      <c r="CW34" s="24"/>
-      <c r="CX34" s="24"/>
-      <c r="CY34" s="24"/>
-      <c r="CZ34" s="24"/>
-      <c r="DA34" s="24"/>
-      <c r="DB34" s="24"/>
-      <c r="DC34" s="24"/>
-      <c r="DD34" s="24"/>
-      <c r="DE34" s="24"/>
-      <c r="DF34" s="24"/>
-      <c r="DG34" s="24"/>
-      <c r="DH34" s="24"/>
-      <c r="DI34" s="24"/>
-      <c r="DJ34" s="24"/>
-      <c r="DK34" s="24"/>
-      <c r="DL34" s="24"/>
-      <c r="DM34" s="24"/>
-    </row>
-    <row r="35" spans="1:117" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="39" t="s">
-        <v>29</v>
-      </c>
-      <c r="B35" s="40">
-        <v>34</v>
+      <c r="T34" s="23"/>
+      <c r="U34" s="23"/>
+      <c r="V34" s="23"/>
+      <c r="W34" s="23"/>
+      <c r="X34" s="23"/>
+      <c r="Y34" s="23"/>
+      <c r="Z34" s="23"/>
+      <c r="AA34" s="23"/>
+      <c r="AB34" s="23"/>
+      <c r="AC34" s="23"/>
+      <c r="AD34" s="23"/>
+      <c r="AE34" s="23"/>
+      <c r="AF34" s="23"/>
+      <c r="AG34" s="23"/>
+      <c r="AH34" s="23"/>
+      <c r="AI34" s="23"/>
+      <c r="AJ34" s="23"/>
+      <c r="AK34" s="23"/>
+      <c r="AL34" s="23"/>
+      <c r="AM34" s="23"/>
+      <c r="AN34" s="23"/>
+      <c r="AO34" s="23"/>
+      <c r="AP34" s="23"/>
+      <c r="AQ34" s="23"/>
+      <c r="AR34" s="23"/>
+      <c r="AS34" s="23"/>
+      <c r="AT34" s="23"/>
+      <c r="AU34" s="23"/>
+      <c r="AV34" s="23"/>
+      <c r="AW34" s="23"/>
+      <c r="AX34" s="23"/>
+      <c r="AY34" s="23"/>
+      <c r="AZ34" s="23"/>
+      <c r="BA34" s="23"/>
+      <c r="BB34" s="23"/>
+      <c r="BC34" s="23"/>
+      <c r="BD34" s="23"/>
+      <c r="BE34" s="23"/>
+      <c r="BF34" s="23"/>
+      <c r="BG34" s="23"/>
+      <c r="BH34" s="23"/>
+      <c r="BI34" s="23"/>
+      <c r="BJ34" s="23"/>
+      <c r="BK34" s="23"/>
+      <c r="BL34" s="23"/>
+      <c r="BM34" s="23"/>
+      <c r="BN34" s="23"/>
+      <c r="BO34" s="23"/>
+      <c r="BP34" s="23"/>
+      <c r="BQ34" s="23"/>
+      <c r="BR34" s="23"/>
+      <c r="BS34" s="23"/>
+      <c r="BT34" s="23"/>
+      <c r="BU34" s="23"/>
+      <c r="BV34" s="23"/>
+      <c r="BW34" s="23"/>
+      <c r="BX34" s="23"/>
+      <c r="BY34" s="23"/>
+      <c r="BZ34" s="23"/>
+      <c r="CA34" s="23"/>
+      <c r="CB34" s="23"/>
+      <c r="CC34" s="23"/>
+      <c r="CD34" s="23"/>
+      <c r="CE34" s="23"/>
+      <c r="CF34" s="23"/>
+      <c r="CG34" s="23"/>
+      <c r="CH34" s="23"/>
+      <c r="CI34" s="23"/>
+      <c r="CJ34" s="23"/>
+      <c r="CK34" s="23"/>
+      <c r="CL34" s="23"/>
+      <c r="CM34" s="23"/>
+      <c r="CN34" s="23"/>
+      <c r="CO34" s="23"/>
+      <c r="CP34" s="23"/>
+      <c r="CQ34" s="23"/>
+      <c r="CR34" s="23"/>
+      <c r="CS34" s="23"/>
+      <c r="CT34" s="23"/>
+      <c r="CU34" s="23"/>
+      <c r="CV34" s="23"/>
+      <c r="CW34" s="23"/>
+      <c r="CX34" s="23"/>
+      <c r="CY34" s="23"/>
+      <c r="CZ34" s="23"/>
+      <c r="DA34" s="23"/>
+      <c r="DB34" s="23"/>
+      <c r="DC34" s="23"/>
+      <c r="DD34" s="23"/>
+      <c r="DE34" s="23"/>
+      <c r="DF34" s="23"/>
+      <c r="DG34" s="23"/>
+      <c r="DH34" s="23"/>
+      <c r="DI34" s="23"/>
+      <c r="DJ34" s="23"/>
+      <c r="DK34" s="23"/>
+      <c r="DL34" s="23"/>
+      <c r="DM34" s="23"/>
+    </row>
+    <row r="35" spans="1:117" s="12" customFormat="1">
+      <c r="A35" s="41" t="s">
+        <v>28</v>
+      </c>
+      <c r="B35" s="42">
+        <v>35</v>
       </c>
       <c r="C35" s="49"/>
       <c r="D35" s="49"/>
       <c r="E35" s="56"/>
-      <c r="F35" s="49"/>
-      <c r="G35" s="49"/>
+      <c r="F35" s="48"/>
+      <c r="G35" s="48"/>
       <c r="H35" s="49"/>
       <c r="I35" s="49"/>
       <c r="J35" s="49"/>
@@ -5485,111 +5476,111 @@
       <c r="Q35" s="18"/>
       <c r="R35" s="18"/>
       <c r="S35" s="18"/>
-      <c r="T35" s="23"/>
-      <c r="U35" s="23"/>
-      <c r="V35" s="23"/>
-      <c r="W35" s="23"/>
-      <c r="X35" s="23"/>
-      <c r="Y35" s="23"/>
-      <c r="Z35" s="23"/>
-      <c r="AA35" s="23"/>
-      <c r="AB35" s="23"/>
-      <c r="AC35" s="23"/>
-      <c r="AD35" s="23"/>
-      <c r="AE35" s="23"/>
-      <c r="AF35" s="23"/>
-      <c r="AG35" s="23"/>
-      <c r="AH35" s="23"/>
-      <c r="AI35" s="23"/>
-      <c r="AJ35" s="23"/>
-      <c r="AK35" s="23"/>
-      <c r="AL35" s="23"/>
-      <c r="AM35" s="23"/>
-      <c r="AN35" s="23"/>
-      <c r="AO35" s="23"/>
-      <c r="AP35" s="23"/>
-      <c r="AQ35" s="23"/>
-      <c r="AR35" s="23"/>
-      <c r="AS35" s="23"/>
-      <c r="AT35" s="23"/>
-      <c r="AU35" s="23"/>
-      <c r="AV35" s="23"/>
-      <c r="AW35" s="23"/>
-      <c r="AX35" s="23"/>
-      <c r="AY35" s="23"/>
-      <c r="AZ35" s="23"/>
-      <c r="BA35" s="23"/>
-      <c r="BB35" s="23"/>
-      <c r="BC35" s="23"/>
-      <c r="BD35" s="23"/>
-      <c r="BE35" s="23"/>
-      <c r="BF35" s="23"/>
-      <c r="BG35" s="23"/>
-      <c r="BH35" s="23"/>
-      <c r="BI35" s="23"/>
-      <c r="BJ35" s="23"/>
-      <c r="BK35" s="23"/>
-      <c r="BL35" s="23"/>
-      <c r="BM35" s="23"/>
-      <c r="BN35" s="23"/>
-      <c r="BO35" s="23"/>
-      <c r="BP35" s="23"/>
-      <c r="BQ35" s="23"/>
-      <c r="BR35" s="23"/>
-      <c r="BS35" s="23"/>
-      <c r="BT35" s="23"/>
-      <c r="BU35" s="23"/>
-      <c r="BV35" s="23"/>
-      <c r="BW35" s="23"/>
-      <c r="BX35" s="23"/>
-      <c r="BY35" s="23"/>
-      <c r="BZ35" s="23"/>
-      <c r="CA35" s="23"/>
-      <c r="CB35" s="23"/>
-      <c r="CC35" s="23"/>
-      <c r="CD35" s="23"/>
-      <c r="CE35" s="23"/>
-      <c r="CF35" s="23"/>
-      <c r="CG35" s="23"/>
-      <c r="CH35" s="23"/>
-      <c r="CI35" s="23"/>
-      <c r="CJ35" s="23"/>
-      <c r="CK35" s="23"/>
-      <c r="CL35" s="23"/>
-      <c r="CM35" s="23"/>
-      <c r="CN35" s="23"/>
-      <c r="CO35" s="23"/>
-      <c r="CP35" s="23"/>
-      <c r="CQ35" s="23"/>
-      <c r="CR35" s="23"/>
-      <c r="CS35" s="23"/>
-      <c r="CT35" s="23"/>
-      <c r="CU35" s="23"/>
-      <c r="CV35" s="23"/>
-      <c r="CW35" s="23"/>
-      <c r="CX35" s="23"/>
-      <c r="CY35" s="23"/>
-      <c r="CZ35" s="23"/>
-      <c r="DA35" s="23"/>
-      <c r="DB35" s="23"/>
-      <c r="DC35" s="23"/>
-      <c r="DD35" s="23"/>
-      <c r="DE35" s="23"/>
-      <c r="DF35" s="23"/>
-      <c r="DG35" s="23"/>
-      <c r="DH35" s="23"/>
-      <c r="DI35" s="23"/>
-      <c r="DJ35" s="23"/>
-      <c r="DK35" s="23"/>
-      <c r="DL35" s="23"/>
-      <c r="DM35" s="23"/>
-    </row>
-    <row r="36" spans="1:117" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="T35" s="18"/>
+      <c r="U35" s="18"/>
+      <c r="V35" s="18"/>
+      <c r="W35" s="18"/>
+      <c r="X35" s="18"/>
+      <c r="Y35" s="18"/>
+      <c r="Z35" s="18"/>
+      <c r="AA35" s="18"/>
+      <c r="AB35" s="18"/>
+      <c r="AC35" s="18"/>
+      <c r="AD35" s="18"/>
+      <c r="AE35" s="18"/>
+      <c r="AF35" s="18"/>
+      <c r="AG35" s="18"/>
+      <c r="AH35" s="18"/>
+      <c r="AI35" s="18"/>
+      <c r="AJ35" s="18"/>
+      <c r="AK35" s="18"/>
+      <c r="AL35" s="18"/>
+      <c r="AM35" s="18"/>
+      <c r="AN35" s="18"/>
+      <c r="AO35" s="18"/>
+      <c r="AP35" s="18"/>
+      <c r="AQ35" s="18"/>
+      <c r="AR35" s="18"/>
+      <c r="AS35" s="18"/>
+      <c r="AT35" s="18"/>
+      <c r="AU35" s="18"/>
+      <c r="AV35" s="18"/>
+      <c r="AW35" s="18"/>
+      <c r="AX35" s="18"/>
+      <c r="AY35" s="18"/>
+      <c r="AZ35" s="18"/>
+      <c r="BA35" s="18"/>
+      <c r="BB35" s="18"/>
+      <c r="BC35" s="18"/>
+      <c r="BD35" s="18"/>
+      <c r="BE35" s="18"/>
+      <c r="BF35" s="18"/>
+      <c r="BG35" s="18"/>
+      <c r="BH35" s="18"/>
+      <c r="BI35" s="18"/>
+      <c r="BJ35" s="18"/>
+      <c r="BK35" s="18"/>
+      <c r="BL35" s="18"/>
+      <c r="BM35" s="18"/>
+      <c r="BN35" s="18"/>
+      <c r="BO35" s="18"/>
+      <c r="BP35" s="18"/>
+      <c r="BQ35" s="18"/>
+      <c r="BR35" s="18"/>
+      <c r="BS35" s="18"/>
+      <c r="BT35" s="18"/>
+      <c r="BU35" s="18"/>
+      <c r="BV35" s="18"/>
+      <c r="BW35" s="18"/>
+      <c r="BX35" s="18"/>
+      <c r="BY35" s="18"/>
+      <c r="BZ35" s="18"/>
+      <c r="CA35" s="18"/>
+      <c r="CB35" s="18"/>
+      <c r="CC35" s="18"/>
+      <c r="CD35" s="18"/>
+      <c r="CE35" s="18"/>
+      <c r="CF35" s="18"/>
+      <c r="CG35" s="18"/>
+      <c r="CH35" s="18"/>
+      <c r="CI35" s="18"/>
+      <c r="CJ35" s="18"/>
+      <c r="CK35" s="18"/>
+      <c r="CL35" s="18"/>
+      <c r="CM35" s="18"/>
+      <c r="CN35" s="18"/>
+      <c r="CO35" s="18"/>
+      <c r="CP35" s="18"/>
+      <c r="CQ35" s="18"/>
+      <c r="CR35" s="18"/>
+      <c r="CS35" s="18"/>
+      <c r="CT35" s="18"/>
+      <c r="CU35" s="18"/>
+      <c r="CV35" s="18"/>
+      <c r="CW35" s="18"/>
+      <c r="CX35" s="18"/>
+      <c r="CY35" s="18"/>
+      <c r="CZ35" s="18"/>
+      <c r="DA35" s="18"/>
+      <c r="DB35" s="18"/>
+      <c r="DC35" s="18"/>
+      <c r="DD35" s="18"/>
+      <c r="DE35" s="18"/>
+      <c r="DF35" s="18"/>
+      <c r="DG35" s="18"/>
+      <c r="DH35" s="18"/>
+      <c r="DI35" s="18"/>
+      <c r="DJ35" s="18"/>
+      <c r="DK35" s="18"/>
+      <c r="DL35" s="18"/>
+      <c r="DM35" s="18"/>
+    </row>
+    <row r="36" spans="1:117" s="12" customFormat="1">
       <c r="A36" s="41" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B36" s="42">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C36" s="49"/>
       <c r="D36" s="49"/>
@@ -5602,7 +5593,7 @@
       <c r="K36" s="18"/>
       <c r="L36" s="18"/>
       <c r="M36" s="49"/>
-      <c r="N36" s="49"/>
+      <c r="N36" s="48"/>
       <c r="O36" s="49"/>
       <c r="P36" s="18"/>
       <c r="Q36" s="18"/>
@@ -5707,30 +5698,30 @@
       <c r="DL36" s="18"/>
       <c r="DM36" s="18"/>
     </row>
-    <row r="37" spans="1:117" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:117" s="12" customFormat="1">
       <c r="A37" s="41" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B37" s="42">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C37" s="49"/>
       <c r="D37" s="49"/>
       <c r="E37" s="56"/>
-      <c r="F37" s="48"/>
-      <c r="G37" s="48"/>
+      <c r="F37" s="49"/>
+      <c r="G37" s="49"/>
       <c r="H37" s="49"/>
       <c r="I37" s="49"/>
-      <c r="J37" s="49"/>
+      <c r="J37" s="59"/>
       <c r="K37" s="18"/>
-      <c r="L37" s="18"/>
-      <c r="M37" s="49"/>
-      <c r="N37" s="48"/>
+      <c r="L37" s="31"/>
+      <c r="M37" s="48"/>
+      <c r="N37" s="49"/>
       <c r="O37" s="49"/>
       <c r="P37" s="18"/>
-      <c r="Q37" s="18"/>
-      <c r="R37" s="18"/>
-      <c r="S37" s="18"/>
+      <c r="Q37" s="31"/>
+      <c r="R37" s="32"/>
+      <c r="S37" s="31"/>
       <c r="T37" s="18"/>
       <c r="U37" s="18"/>
       <c r="V37" s="18"/>
@@ -5830,30 +5821,30 @@
       <c r="DL37" s="18"/>
       <c r="DM37" s="18"/>
     </row>
-    <row r="38" spans="1:117" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:117" s="12" customFormat="1">
       <c r="A38" s="41" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B38" s="42">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C38" s="49"/>
       <c r="D38" s="49"/>
-      <c r="E38" s="56"/>
-      <c r="F38" s="49"/>
-      <c r="G38" s="49"/>
-      <c r="H38" s="49"/>
+      <c r="E38" s="55"/>
+      <c r="F38" s="48"/>
+      <c r="G38" s="48"/>
+      <c r="H38" s="48"/>
       <c r="I38" s="49"/>
-      <c r="J38" s="59"/>
-      <c r="K38" s="18"/>
-      <c r="L38" s="31"/>
-      <c r="M38" s="48"/>
-      <c r="N38" s="49"/>
+      <c r="J38" s="49"/>
+      <c r="K38" s="32"/>
+      <c r="L38" s="18"/>
+      <c r="M38" s="49"/>
+      <c r="N38" s="48"/>
       <c r="O38" s="49"/>
-      <c r="P38" s="18"/>
-      <c r="Q38" s="31"/>
-      <c r="R38" s="32"/>
-      <c r="S38" s="31"/>
+      <c r="P38" s="32"/>
+      <c r="Q38" s="33"/>
+      <c r="R38" s="33"/>
+      <c r="S38" s="18"/>
       <c r="T38" s="18"/>
       <c r="U38" s="18"/>
       <c r="V38" s="18"/>
@@ -5953,30 +5944,30 @@
       <c r="DL38" s="18"/>
       <c r="DM38" s="18"/>
     </row>
-    <row r="39" spans="1:117" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:117" s="12" customFormat="1">
       <c r="A39" s="41" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B39" s="42">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C39" s="49"/>
       <c r="D39" s="49"/>
-      <c r="E39" s="55"/>
-      <c r="F39" s="48"/>
-      <c r="G39" s="48"/>
+      <c r="E39" s="56"/>
+      <c r="F39" s="49"/>
+      <c r="G39" s="49"/>
       <c r="H39" s="48"/>
-      <c r="I39" s="49"/>
-      <c r="J39" s="49"/>
-      <c r="K39" s="32"/>
-      <c r="L39" s="18"/>
-      <c r="M39" s="49"/>
-      <c r="N39" s="48"/>
-      <c r="O39" s="49"/>
-      <c r="P39" s="32"/>
-      <c r="Q39" s="33"/>
-      <c r="R39" s="33"/>
-      <c r="S39" s="18"/>
+      <c r="I39" s="48"/>
+      <c r="J39" s="48"/>
+      <c r="K39" s="31"/>
+      <c r="L39" s="31"/>
+      <c r="M39" s="48"/>
+      <c r="N39" s="49"/>
+      <c r="O39" s="48"/>
+      <c r="P39" s="31"/>
+      <c r="Q39" s="31"/>
+      <c r="R39" s="31"/>
+      <c r="S39" s="31"/>
       <c r="T39" s="18"/>
       <c r="U39" s="18"/>
       <c r="V39" s="18"/>
@@ -6076,29 +6067,29 @@
       <c r="DL39" s="18"/>
       <c r="DM39" s="18"/>
     </row>
-    <row r="40" spans="1:117" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:117" s="12" customFormat="1">
       <c r="A40" s="41" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B40" s="42">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C40" s="49"/>
       <c r="D40" s="49"/>
-      <c r="E40" s="56"/>
+      <c r="E40" s="55"/>
       <c r="F40" s="49"/>
       <c r="G40" s="49"/>
       <c r="H40" s="48"/>
       <c r="I40" s="48"/>
       <c r="J40" s="48"/>
       <c r="K40" s="31"/>
-      <c r="L40" s="31"/>
+      <c r="L40" s="18"/>
       <c r="M40" s="48"/>
-      <c r="N40" s="49"/>
+      <c r="N40" s="48"/>
       <c r="O40" s="48"/>
       <c r="P40" s="31"/>
       <c r="Q40" s="31"/>
-      <c r="R40" s="31"/>
+      <c r="R40" s="32"/>
       <c r="S40" s="31"/>
       <c r="T40" s="18"/>
       <c r="U40" s="18"/>
@@ -6199,30 +6190,30 @@
       <c r="DL40" s="18"/>
       <c r="DM40" s="18"/>
     </row>
-    <row r="41" spans="1:117" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:117" s="12" customFormat="1">
       <c r="A41" s="41" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B41" s="42">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C41" s="49"/>
       <c r="D41" s="49"/>
-      <c r="E41" s="55"/>
+      <c r="E41" s="56"/>
       <c r="F41" s="49"/>
       <c r="G41" s="49"/>
-      <c r="H41" s="48"/>
-      <c r="I41" s="48"/>
-      <c r="J41" s="48"/>
-      <c r="K41" s="31"/>
-      <c r="L41" s="18"/>
-      <c r="M41" s="48"/>
-      <c r="N41" s="48"/>
-      <c r="O41" s="48"/>
-      <c r="P41" s="31"/>
-      <c r="Q41" s="31"/>
-      <c r="R41" s="32"/>
-      <c r="S41" s="31"/>
+      <c r="H41" s="49"/>
+      <c r="I41" s="49"/>
+      <c r="J41" s="49"/>
+      <c r="K41" s="18"/>
+      <c r="L41" s="31"/>
+      <c r="M41" s="49"/>
+      <c r="N41" s="49"/>
+      <c r="O41" s="49"/>
+      <c r="P41" s="18"/>
+      <c r="Q41" s="18"/>
+      <c r="R41" s="18"/>
+      <c r="S41" s="18"/>
       <c r="T41" s="18"/>
       <c r="U41" s="18"/>
       <c r="V41" s="18"/>
@@ -6322,30 +6313,30 @@
       <c r="DL41" s="18"/>
       <c r="DM41" s="18"/>
     </row>
-    <row r="42" spans="1:117" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:117" s="12" customFormat="1">
       <c r="A42" s="41" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B42" s="42">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C42" s="49"/>
       <c r="D42" s="49"/>
-      <c r="E42" s="56"/>
+      <c r="E42" s="55"/>
       <c r="F42" s="49"/>
       <c r="G42" s="49"/>
-      <c r="H42" s="49"/>
-      <c r="I42" s="49"/>
-      <c r="J42" s="49"/>
-      <c r="K42" s="18"/>
+      <c r="H42" s="48"/>
+      <c r="I42" s="48"/>
+      <c r="J42" s="48"/>
+      <c r="K42" s="31"/>
       <c r="L42" s="31"/>
-      <c r="M42" s="49"/>
+      <c r="M42" s="48"/>
       <c r="N42" s="49"/>
-      <c r="O42" s="49"/>
-      <c r="P42" s="18"/>
-      <c r="Q42" s="18"/>
-      <c r="R42" s="18"/>
-      <c r="S42" s="18"/>
+      <c r="O42" s="48"/>
+      <c r="P42" s="31"/>
+      <c r="Q42" s="31"/>
+      <c r="R42" s="31"/>
+      <c r="S42" s="31"/>
       <c r="T42" s="18"/>
       <c r="U42" s="18"/>
       <c r="V42" s="18"/>
@@ -6445,290 +6436,167 @@
       <c r="DL42" s="18"/>
       <c r="DM42" s="18"/>
     </row>
-    <row r="43" spans="1:117" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="41" t="s">
-        <v>37</v>
-      </c>
-      <c r="B43" s="42">
-        <v>42</v>
+    <row r="43" spans="1:117" s="15" customFormat="1" ht="12" thickBot="1">
+      <c r="A43" s="43" t="s">
+        <v>36</v>
+      </c>
+      <c r="B43" s="44">
+        <v>43</v>
       </c>
       <c r="C43" s="49"/>
       <c r="D43" s="49"/>
       <c r="E43" s="55"/>
-      <c r="F43" s="49"/>
-      <c r="G43" s="49"/>
+      <c r="F43" s="48"/>
+      <c r="G43" s="48"/>
       <c r="H43" s="48"/>
       <c r="I43" s="48"/>
       <c r="J43" s="48"/>
       <c r="K43" s="31"/>
-      <c r="L43" s="31"/>
-      <c r="M43" s="48"/>
+      <c r="L43" s="18"/>
+      <c r="M43" s="49"/>
       <c r="N43" s="49"/>
       <c r="O43" s="48"/>
       <c r="P43" s="31"/>
       <c r="Q43" s="31"/>
       <c r="R43" s="31"/>
-      <c r="S43" s="31"/>
-      <c r="T43" s="18"/>
-      <c r="U43" s="18"/>
-      <c r="V43" s="18"/>
-      <c r="W43" s="18"/>
-      <c r="X43" s="18"/>
-      <c r="Y43" s="18"/>
-      <c r="Z43" s="18"/>
-      <c r="AA43" s="18"/>
-      <c r="AB43" s="18"/>
-      <c r="AC43" s="18"/>
-      <c r="AD43" s="18"/>
-      <c r="AE43" s="18"/>
-      <c r="AF43" s="18"/>
-      <c r="AG43" s="18"/>
-      <c r="AH43" s="18"/>
-      <c r="AI43" s="18"/>
-      <c r="AJ43" s="18"/>
-      <c r="AK43" s="18"/>
-      <c r="AL43" s="18"/>
-      <c r="AM43" s="18"/>
-      <c r="AN43" s="18"/>
-      <c r="AO43" s="18"/>
-      <c r="AP43" s="18"/>
-      <c r="AQ43" s="18"/>
-      <c r="AR43" s="18"/>
-      <c r="AS43" s="18"/>
-      <c r="AT43" s="18"/>
-      <c r="AU43" s="18"/>
-      <c r="AV43" s="18"/>
-      <c r="AW43" s="18"/>
-      <c r="AX43" s="18"/>
-      <c r="AY43" s="18"/>
-      <c r="AZ43" s="18"/>
-      <c r="BA43" s="18"/>
-      <c r="BB43" s="18"/>
-      <c r="BC43" s="18"/>
-      <c r="BD43" s="18"/>
-      <c r="BE43" s="18"/>
-      <c r="BF43" s="18"/>
-      <c r="BG43" s="18"/>
-      <c r="BH43" s="18"/>
-      <c r="BI43" s="18"/>
-      <c r="BJ43" s="18"/>
-      <c r="BK43" s="18"/>
-      <c r="BL43" s="18"/>
-      <c r="BM43" s="18"/>
-      <c r="BN43" s="18"/>
-      <c r="BO43" s="18"/>
-      <c r="BP43" s="18"/>
-      <c r="BQ43" s="18"/>
-      <c r="BR43" s="18"/>
-      <c r="BS43" s="18"/>
-      <c r="BT43" s="18"/>
-      <c r="BU43" s="18"/>
-      <c r="BV43" s="18"/>
-      <c r="BW43" s="18"/>
-      <c r="BX43" s="18"/>
-      <c r="BY43" s="18"/>
-      <c r="BZ43" s="18"/>
-      <c r="CA43" s="18"/>
-      <c r="CB43" s="18"/>
-      <c r="CC43" s="18"/>
-      <c r="CD43" s="18"/>
-      <c r="CE43" s="18"/>
-      <c r="CF43" s="18"/>
-      <c r="CG43" s="18"/>
-      <c r="CH43" s="18"/>
-      <c r="CI43" s="18"/>
-      <c r="CJ43" s="18"/>
-      <c r="CK43" s="18"/>
-      <c r="CL43" s="18"/>
-      <c r="CM43" s="18"/>
-      <c r="CN43" s="18"/>
-      <c r="CO43" s="18"/>
-      <c r="CP43" s="18"/>
-      <c r="CQ43" s="18"/>
-      <c r="CR43" s="18"/>
-      <c r="CS43" s="18"/>
-      <c r="CT43" s="18"/>
-      <c r="CU43" s="18"/>
-      <c r="CV43" s="18"/>
-      <c r="CW43" s="18"/>
-      <c r="CX43" s="18"/>
-      <c r="CY43" s="18"/>
-      <c r="CZ43" s="18"/>
-      <c r="DA43" s="18"/>
-      <c r="DB43" s="18"/>
-      <c r="DC43" s="18"/>
-      <c r="DD43" s="18"/>
-      <c r="DE43" s="18"/>
-      <c r="DF43" s="18"/>
-      <c r="DG43" s="18"/>
-      <c r="DH43" s="18"/>
-      <c r="DI43" s="18"/>
-      <c r="DJ43" s="18"/>
-      <c r="DK43" s="18"/>
-      <c r="DL43" s="18"/>
-      <c r="DM43" s="18"/>
-    </row>
-    <row r="44" spans="1:117" s="15" customFormat="1" ht="12" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="43" t="s">
-        <v>38</v>
-      </c>
-      <c r="B44" s="44">
-        <v>43</v>
-      </c>
-      <c r="C44" s="49"/>
-      <c r="D44" s="49"/>
-      <c r="E44" s="55"/>
-      <c r="F44" s="48"/>
-      <c r="G44" s="48"/>
-      <c r="H44" s="48"/>
-      <c r="I44" s="48"/>
-      <c r="J44" s="48"/>
-      <c r="K44" s="31"/>
-      <c r="L44" s="18"/>
-      <c r="M44" s="49"/>
-      <c r="N44" s="49"/>
-      <c r="O44" s="48"/>
-      <c r="P44" s="31"/>
-      <c r="Q44" s="31"/>
-      <c r="R44" s="31"/>
-      <c r="S44" s="18"/>
-      <c r="T44" s="24"/>
-      <c r="U44" s="24"/>
-      <c r="V44" s="24"/>
-      <c r="W44" s="24"/>
-      <c r="X44" s="24"/>
-      <c r="Y44" s="24"/>
-      <c r="Z44" s="24"/>
-      <c r="AA44" s="24"/>
-      <c r="AB44" s="24"/>
-      <c r="AC44" s="24"/>
-      <c r="AD44" s="24"/>
-      <c r="AE44" s="24"/>
-      <c r="AF44" s="24"/>
-      <c r="AG44" s="24"/>
-      <c r="AH44" s="24"/>
-      <c r="AI44" s="24"/>
-      <c r="AJ44" s="24"/>
-      <c r="AK44" s="24"/>
-      <c r="AL44" s="24"/>
-      <c r="AM44" s="24"/>
-      <c r="AN44" s="24"/>
-      <c r="AO44" s="24"/>
-      <c r="AP44" s="24"/>
-      <c r="AQ44" s="24"/>
-      <c r="AR44" s="24"/>
-      <c r="AS44" s="24"/>
-      <c r="AT44" s="24"/>
-      <c r="AU44" s="24"/>
-      <c r="AV44" s="24"/>
-      <c r="AW44" s="24"/>
-      <c r="AX44" s="24"/>
-      <c r="AY44" s="24"/>
-      <c r="AZ44" s="24"/>
-      <c r="BA44" s="24"/>
-      <c r="BB44" s="24"/>
-      <c r="BC44" s="24"/>
-      <c r="BD44" s="24"/>
-      <c r="BE44" s="24"/>
-      <c r="BF44" s="24"/>
-      <c r="BG44" s="24"/>
-      <c r="BH44" s="24"/>
-      <c r="BI44" s="24"/>
-      <c r="BJ44" s="24"/>
-      <c r="BK44" s="24"/>
-      <c r="BL44" s="24"/>
-      <c r="BM44" s="24"/>
-      <c r="BN44" s="24"/>
-      <c r="BO44" s="24"/>
-      <c r="BP44" s="24"/>
-      <c r="BQ44" s="24"/>
-      <c r="BR44" s="24"/>
-      <c r="BS44" s="24"/>
-      <c r="BT44" s="24"/>
-      <c r="BU44" s="24"/>
-      <c r="BV44" s="24"/>
-      <c r="BW44" s="24"/>
-      <c r="BX44" s="24"/>
-      <c r="BY44" s="24"/>
-      <c r="BZ44" s="24"/>
-      <c r="CA44" s="24"/>
-      <c r="CB44" s="24"/>
-      <c r="CC44" s="24"/>
-      <c r="CD44" s="24"/>
-      <c r="CE44" s="24"/>
-      <c r="CF44" s="24"/>
-      <c r="CG44" s="24"/>
-      <c r="CH44" s="24"/>
-      <c r="CI44" s="24"/>
-      <c r="CJ44" s="24"/>
-      <c r="CK44" s="24"/>
-      <c r="CL44" s="24"/>
-      <c r="CM44" s="24"/>
-      <c r="CN44" s="24"/>
-      <c r="CO44" s="24"/>
-      <c r="CP44" s="24"/>
-      <c r="CQ44" s="24"/>
-      <c r="CR44" s="24"/>
-      <c r="CS44" s="24"/>
-      <c r="CT44" s="24"/>
-      <c r="CU44" s="24"/>
-      <c r="CV44" s="24"/>
-      <c r="CW44" s="24"/>
-      <c r="CX44" s="24"/>
-      <c r="CY44" s="24"/>
-      <c r="CZ44" s="24"/>
-      <c r="DA44" s="24"/>
-      <c r="DB44" s="24"/>
-      <c r="DC44" s="24"/>
-      <c r="DD44" s="24"/>
-      <c r="DE44" s="24"/>
-      <c r="DF44" s="24"/>
-      <c r="DG44" s="24"/>
-      <c r="DH44" s="24"/>
-      <c r="DI44" s="24"/>
-      <c r="DJ44" s="24"/>
-      <c r="DK44" s="24"/>
-      <c r="DL44" s="24"/>
-      <c r="DM44" s="24"/>
-    </row>
-    <row r="45" spans="1:117" x14ac:dyDescent="0.2">
+      <c r="S43" s="18"/>
+      <c r="T43" s="24"/>
+      <c r="U43" s="24"/>
+      <c r="V43" s="24"/>
+      <c r="W43" s="24"/>
+      <c r="X43" s="24"/>
+      <c r="Y43" s="24"/>
+      <c r="Z43" s="24"/>
+      <c r="AA43" s="24"/>
+      <c r="AB43" s="24"/>
+      <c r="AC43" s="24"/>
+      <c r="AD43" s="24"/>
+      <c r="AE43" s="24"/>
+      <c r="AF43" s="24"/>
+      <c r="AG43" s="24"/>
+      <c r="AH43" s="24"/>
+      <c r="AI43" s="24"/>
+      <c r="AJ43" s="24"/>
+      <c r="AK43" s="24"/>
+      <c r="AL43" s="24"/>
+      <c r="AM43" s="24"/>
+      <c r="AN43" s="24"/>
+      <c r="AO43" s="24"/>
+      <c r="AP43" s="24"/>
+      <c r="AQ43" s="24"/>
+      <c r="AR43" s="24"/>
+      <c r="AS43" s="24"/>
+      <c r="AT43" s="24"/>
+      <c r="AU43" s="24"/>
+      <c r="AV43" s="24"/>
+      <c r="AW43" s="24"/>
+      <c r="AX43" s="24"/>
+      <c r="AY43" s="24"/>
+      <c r="AZ43" s="24"/>
+      <c r="BA43" s="24"/>
+      <c r="BB43" s="24"/>
+      <c r="BC43" s="24"/>
+      <c r="BD43" s="24"/>
+      <c r="BE43" s="24"/>
+      <c r="BF43" s="24"/>
+      <c r="BG43" s="24"/>
+      <c r="BH43" s="24"/>
+      <c r="BI43" s="24"/>
+      <c r="BJ43" s="24"/>
+      <c r="BK43" s="24"/>
+      <c r="BL43" s="24"/>
+      <c r="BM43" s="24"/>
+      <c r="BN43" s="24"/>
+      <c r="BO43" s="24"/>
+      <c r="BP43" s="24"/>
+      <c r="BQ43" s="24"/>
+      <c r="BR43" s="24"/>
+      <c r="BS43" s="24"/>
+      <c r="BT43" s="24"/>
+      <c r="BU43" s="24"/>
+      <c r="BV43" s="24"/>
+      <c r="BW43" s="24"/>
+      <c r="BX43" s="24"/>
+      <c r="BY43" s="24"/>
+      <c r="BZ43" s="24"/>
+      <c r="CA43" s="24"/>
+      <c r="CB43" s="24"/>
+      <c r="CC43" s="24"/>
+      <c r="CD43" s="24"/>
+      <c r="CE43" s="24"/>
+      <c r="CF43" s="24"/>
+      <c r="CG43" s="24"/>
+      <c r="CH43" s="24"/>
+      <c r="CI43" s="24"/>
+      <c r="CJ43" s="24"/>
+      <c r="CK43" s="24"/>
+      <c r="CL43" s="24"/>
+      <c r="CM43" s="24"/>
+      <c r="CN43" s="24"/>
+      <c r="CO43" s="24"/>
+      <c r="CP43" s="24"/>
+      <c r="CQ43" s="24"/>
+      <c r="CR43" s="24"/>
+      <c r="CS43" s="24"/>
+      <c r="CT43" s="24"/>
+      <c r="CU43" s="24"/>
+      <c r="CV43" s="24"/>
+      <c r="CW43" s="24"/>
+      <c r="CX43" s="24"/>
+      <c r="CY43" s="24"/>
+      <c r="CZ43" s="24"/>
+      <c r="DA43" s="24"/>
+      <c r="DB43" s="24"/>
+      <c r="DC43" s="24"/>
+      <c r="DD43" s="24"/>
+      <c r="DE43" s="24"/>
+      <c r="DF43" s="24"/>
+      <c r="DG43" s="24"/>
+      <c r="DH43" s="24"/>
+      <c r="DI43" s="24"/>
+      <c r="DJ43" s="24"/>
+      <c r="DK43" s="24"/>
+      <c r="DL43" s="24"/>
+      <c r="DM43" s="24"/>
+    </row>
+    <row r="44" spans="1:117">
+      <c r="A44" s="38"/>
+    </row>
+    <row r="45" spans="1:117">
       <c r="A45" s="38"/>
     </row>
-    <row r="46" spans="1:117" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:117">
       <c r="A46" s="38"/>
     </row>
-    <row r="47" spans="1:117" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:117">
       <c r="A47" s="38"/>
     </row>
-    <row r="48" spans="1:117" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:117">
       <c r="A48" s="38"/>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:1">
       <c r="A49" s="38"/>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:1">
       <c r="A50" s="38"/>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:1">
       <c r="A51" s="38"/>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:1">
       <c r="A52" s="38"/>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:1">
       <c r="A53" s="38"/>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:1">
       <c r="A54" s="38"/>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:1">
       <c r="A55" s="38"/>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:1">
       <c r="A56" s="38"/>
-    </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A57" s="38"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>